<commit_message>
update: update XRO fcst 2024-10
</commit_message>
<xml_diff>
--- a/content/climate/XRO/XRO_ENSO_fcst.xlsx
+++ b/content/climate/XRO/XRO_ENSO_fcst.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>init</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>2024-08</t>
+  </si>
+  <si>
+    <t>2024-09</t>
   </si>
   <si>
     <t>Readme</t>
@@ -454,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,7 +468,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2">
         <v>0</v>
@@ -1644,58 +1647,58 @@
         <v>0.067</v>
       </c>
       <c r="D19" s="1">
-        <v>-0.177</v>
+        <v>-0.178</v>
       </c>
       <c r="E19" s="1">
-        <v>-0.326</v>
+        <v>-0.327</v>
       </c>
       <c r="F19" s="1">
-        <v>-0.483</v>
+        <v>-0.484</v>
       </c>
       <c r="G19" s="1">
-        <v>-0.658</v>
+        <v>-0.659</v>
       </c>
       <c r="H19" s="1">
-        <v>-0.783</v>
+        <v>-0.785</v>
       </c>
       <c r="I19" s="1">
-        <v>-0.794</v>
+        <v>-0.796</v>
       </c>
       <c r="J19" s="1">
-        <v>-0.708</v>
+        <v>-0.709</v>
       </c>
       <c r="K19" s="1">
-        <v>-0.61</v>
+        <v>-0.611</v>
       </c>
       <c r="L19" s="1">
+        <v>-0.555</v>
+      </c>
+      <c r="M19" s="1">
         <v>-0.554</v>
       </c>
-      <c r="M19" s="1">
-        <v>-0.553</v>
-      </c>
       <c r="N19" s="1">
-        <v>-0.586</v>
+        <v>-0.587</v>
       </c>
       <c r="O19" s="1">
-        <v>-0.603</v>
+        <v>-0.604</v>
       </c>
       <c r="P19" s="1">
-        <v>-0.577</v>
+        <v>-0.578</v>
       </c>
       <c r="Q19" s="1">
-        <v>-0.539</v>
+        <v>-0.54</v>
       </c>
       <c r="R19" s="1">
         <v>-0.541</v>
       </c>
       <c r="S19" s="1">
-        <v>-0.598</v>
+        <v>-0.599</v>
       </c>
       <c r="T19" s="1">
-        <v>-0.668</v>
+        <v>-0.669</v>
       </c>
       <c r="U19" s="1">
-        <v>-0.6850000000000001</v>
+        <v>-0.6860000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -1706,61 +1709,61 @@
         <v>0.192</v>
       </c>
       <c r="C20" s="1">
-        <v>0.073</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D20" s="1">
-        <v>-0.114</v>
+        <v>-0.118</v>
       </c>
       <c r="E20" s="1">
-        <v>-0.298</v>
+        <v>-0.304</v>
       </c>
       <c r="F20" s="1">
-        <v>-0.465</v>
+        <v>-0.473</v>
       </c>
       <c r="G20" s="1">
+        <v>-0.5669999999999999</v>
+      </c>
+      <c r="H20" s="1">
         <v>-0.5570000000000001</v>
       </c>
-      <c r="H20" s="1">
-        <v>-0.547</v>
-      </c>
       <c r="I20" s="1">
-        <v>-0.471</v>
+        <v>-0.481</v>
       </c>
       <c r="J20" s="1">
-        <v>-0.403</v>
+        <v>-0.411</v>
       </c>
       <c r="K20" s="1">
-        <v>-0.378</v>
+        <v>-0.385</v>
       </c>
       <c r="L20" s="1">
-        <v>-0.4</v>
+        <v>-0.407</v>
       </c>
       <c r="M20" s="1">
-        <v>-0.453</v>
+        <v>-0.46</v>
       </c>
       <c r="N20" s="1">
-        <v>-0.493</v>
+        <v>-0.5</v>
       </c>
       <c r="O20" s="1">
-        <v>-0.49</v>
+        <v>-0.497</v>
       </c>
       <c r="P20" s="1">
-        <v>-0.47</v>
+        <v>-0.476</v>
       </c>
       <c r="Q20" s="1">
-        <v>-0.479</v>
+        <v>-0.485</v>
       </c>
       <c r="R20" s="1">
-        <v>-0.532</v>
+        <v>-0.538</v>
       </c>
       <c r="S20" s="1">
-        <v>-0.594</v>
+        <v>-0.601</v>
       </c>
       <c r="T20" s="1">
-        <v>-0.607</v>
+        <v>-0.614</v>
       </c>
       <c r="U20" s="1">
-        <v>-0.553</v>
+        <v>-0.5590000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -1768,64 +1771,129 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>-0.07199999999999999</v>
+        <v>-0.051</v>
       </c>
       <c r="C21" s="1">
-        <v>-0.154</v>
+        <v>-0.137</v>
       </c>
       <c r="D21" s="1">
-        <v>-0.313</v>
+        <v>-0.301</v>
       </c>
       <c r="E21" s="1">
+        <v>-0.458</v>
+      </c>
+      <c r="F21" s="1">
+        <v>-0.551</v>
+      </c>
+      <c r="G21" s="1">
+        <v>-0.542</v>
+      </c>
+      <c r="H21" s="1">
         <v>-0.468</v>
       </c>
-      <c r="F21" s="1">
-        <v>-0.5590000000000001</v>
-      </c>
-      <c r="G21" s="1">
-        <v>-0.55</v>
-      </c>
-      <c r="H21" s="1">
-        <v>-0.475</v>
-      </c>
       <c r="I21" s="1">
-        <v>-0.412</v>
+        <v>-0.409</v>
       </c>
       <c r="J21" s="1">
         <v>-0.404</v>
       </c>
       <c r="K21" s="1">
-        <v>-0.459</v>
+        <v>-0.463</v>
       </c>
       <c r="L21" s="1">
-        <v>-0.554</v>
+        <v>-0.5649999999999999</v>
       </c>
       <c r="M21" s="1">
-        <v>-0.626</v>
+        <v>-0.642</v>
       </c>
       <c r="N21" s="1">
+        <v>-0.648</v>
+      </c>
+      <c r="O21" s="1">
+        <v>-0.623</v>
+      </c>
+      <c r="P21" s="1">
+        <v>-0.639</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>-0.718</v>
+      </c>
+      <c r="R21" s="1">
+        <v>-0.8110000000000001</v>
+      </c>
+      <c r="S21" s="1">
+        <v>-0.834</v>
+      </c>
+      <c r="T21" s="1">
+        <v>-0.759</v>
+      </c>
+      <c r="U21" s="1">
+        <v>-0.632</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>-0.236</v>
+      </c>
+      <c r="C22" s="1">
+        <v>-0.324</v>
+      </c>
+      <c r="D22" s="1">
+        <v>-0.465</v>
+      </c>
+      <c r="E22" s="1">
+        <v>-0.532</v>
+      </c>
+      <c r="F22" s="1">
+        <v>-0.505</v>
+      </c>
+      <c r="G22" s="1">
+        <v>-0.431</v>
+      </c>
+      <c r="H22" s="1">
+        <v>-0.383</v>
+      </c>
+      <c r="I22" s="1">
+        <v>-0.389</v>
+      </c>
+      <c r="J22" s="1">
+        <v>-0.452</v>
+      </c>
+      <c r="K22" s="1">
+        <v>-0.552</v>
+      </c>
+      <c r="L22" s="1">
+        <v>-0.628</v>
+      </c>
+      <c r="M22" s="1">
+        <v>-0.636</v>
+      </c>
+      <c r="N22" s="1">
+        <v>-0.614</v>
+      </c>
+      <c r="O22" s="1">
         <v>-0.631</v>
       </c>
-      <c r="O21" s="1">
-        <v>-0.606</v>
-      </c>
-      <c r="P21" s="1">
-        <v>-0.62</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>-0.697</v>
-      </c>
-      <c r="R21" s="1">
-        <v>-0.787</v>
-      </c>
-      <c r="S21" s="1">
-        <v>-0.8080000000000001</v>
-      </c>
-      <c r="T21" s="1">
-        <v>-0.736</v>
-      </c>
-      <c r="U21" s="1">
-        <v>-0.613</v>
+      <c r="P22" s="1">
+        <v>-0.707</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>-0.793</v>
+      </c>
+      <c r="R22" s="1">
+        <v>-0.8110000000000001</v>
+      </c>
+      <c r="S22" s="1">
+        <v>-0.737</v>
+      </c>
+      <c r="T22" s="1">
+        <v>-0.615</v>
+      </c>
+      <c r="U22" s="1">
+        <v>-0.484</v>
       </c>
     </row>
   </sheetData>
@@ -1843,22 +1911,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: update XRO fcsts
</commit_message>
<xml_diff>
--- a/content/climate/XRO/XRO_ENSO_fcst.xlsx
+++ b/content/climate/XRO/XRO_ENSO_fcst.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>init</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>2024-09</t>
+  </si>
+  <si>
+    <t>2024-10</t>
   </si>
   <si>
     <t>Readme</t>
@@ -457,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -468,7 +471,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2">
         <v>0</v>
@@ -1792,7 +1795,7 @@
         <v>-0.468</v>
       </c>
       <c r="I21" s="1">
-        <v>-0.409</v>
+        <v>-0.408</v>
       </c>
       <c r="J21" s="1">
         <v>-0.404</v>
@@ -1813,7 +1816,7 @@
         <v>-0.623</v>
       </c>
       <c r="P21" s="1">
-        <v>-0.639</v>
+        <v>-0.638</v>
       </c>
       <c r="Q21" s="1">
         <v>-0.718</v>
@@ -1836,64 +1839,129 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>-0.236</v>
+        <v>-0.217</v>
       </c>
       <c r="C22" s="1">
-        <v>-0.324</v>
+        <v>-0.295</v>
       </c>
       <c r="D22" s="1">
-        <v>-0.465</v>
+        <v>-0.427</v>
       </c>
       <c r="E22" s="1">
-        <v>-0.532</v>
+        <v>-0.498</v>
       </c>
       <c r="F22" s="1">
-        <v>-0.505</v>
+        <v>-0.482</v>
       </c>
       <c r="G22" s="1">
-        <v>-0.431</v>
+        <v>-0.419</v>
       </c>
       <c r="H22" s="1">
-        <v>-0.383</v>
+        <v>-0.38</v>
       </c>
       <c r="I22" s="1">
-        <v>-0.389</v>
+        <v>-0.397</v>
       </c>
       <c r="J22" s="1">
-        <v>-0.452</v>
+        <v>-0.476</v>
       </c>
       <c r="K22" s="1">
-        <v>-0.552</v>
+        <v>-0.597</v>
       </c>
       <c r="L22" s="1">
-        <v>-0.628</v>
+        <v>-0.6899999999999999</v>
       </c>
       <c r="M22" s="1">
-        <v>-0.636</v>
+        <v>-0.702</v>
       </c>
       <c r="N22" s="1">
-        <v>-0.614</v>
+        <v>-0.679</v>
       </c>
       <c r="O22" s="1">
-        <v>-0.631</v>
+        <v>-0.7</v>
       </c>
       <c r="P22" s="1">
-        <v>-0.707</v>
+        <v>-0.792</v>
       </c>
       <c r="Q22" s="1">
-        <v>-0.793</v>
+        <v>-0.897</v>
       </c>
       <c r="R22" s="1">
-        <v>-0.8110000000000001</v>
+        <v>-0.922</v>
       </c>
       <c r="S22" s="1">
-        <v>-0.737</v>
+        <v>-0.839</v>
       </c>
       <c r="T22" s="1">
-        <v>-0.615</v>
+        <v>-0.7</v>
       </c>
       <c r="U22" s="1">
+        <v>-0.555</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>-0.283</v>
+      </c>
+      <c r="C23" s="1">
+        <v>-0.369</v>
+      </c>
+      <c r="D23" s="1">
+        <v>-0.43</v>
+      </c>
+      <c r="E23" s="1">
+        <v>-0.376</v>
+      </c>
+      <c r="F23" s="1">
+        <v>-0.293</v>
+      </c>
+      <c r="G23" s="1">
+        <v>-0.258</v>
+      </c>
+      <c r="H23" s="1">
+        <v>-0.287</v>
+      </c>
+      <c r="I23" s="1">
+        <v>-0.369</v>
+      </c>
+      <c r="J23" s="1">
         <v>-0.484</v>
+      </c>
+      <c r="K23" s="1">
+        <v>-0.575</v>
+      </c>
+      <c r="L23" s="1">
+        <v>-0.596</v>
+      </c>
+      <c r="M23" s="1">
+        <v>-0.582</v>
+      </c>
+      <c r="N23" s="1">
+        <v>-0.603</v>
+      </c>
+      <c r="O23" s="1">
+        <v>-0.68</v>
+      </c>
+      <c r="P23" s="1">
+        <v>-0.764</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>-0.781</v>
+      </c>
+      <c r="R23" s="1">
+        <v>-0.709</v>
+      </c>
+      <c r="S23" s="1">
+        <v>-0.592</v>
+      </c>
+      <c r="T23" s="1">
+        <v>-0.469</v>
+      </c>
+      <c r="U23" s="1">
+        <v>-0.342</v>
       </c>
     </row>
   </sheetData>
@@ -1911,22 +1979,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: XRO forecast 2025/05
</commit_message>
<xml_diff>
--- a/content/climate/XRO/XRO_ENSO_fcst.xlsx
+++ b/content/climate/XRO/XRO_ENSO_fcst.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>init</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>2025-03</t>
+  </si>
+  <si>
+    <t>2025-04</t>
   </si>
   <si>
     <t>Readme</t>
@@ -475,7 +478,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,7 +489,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2">
         <v>0</v>
@@ -2126,52 +2129,52 @@
         <v>-0.49</v>
       </c>
       <c r="F26" s="1">
-        <v>-0.488</v>
+        <v>-0.489</v>
       </c>
       <c r="G26" s="1">
-        <v>-0.506</v>
+        <v>-0.507</v>
       </c>
       <c r="H26" s="1">
-        <v>-0.517</v>
+        <v>-0.518</v>
       </c>
       <c r="I26" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="J26" s="1">
+        <v>-0.47</v>
+      </c>
+      <c r="K26" s="1">
+        <v>-0.467</v>
+      </c>
+      <c r="L26" s="1">
         <v>-0.499</v>
       </c>
-      <c r="J26" s="1">
-        <v>-0.468</v>
-      </c>
-      <c r="K26" s="1">
-        <v>-0.465</v>
-      </c>
-      <c r="L26" s="1">
-        <v>-0.497</v>
-      </c>
       <c r="M26" s="1">
-        <v>-0.524</v>
+        <v>-0.527</v>
       </c>
       <c r="N26" s="1">
-        <v>-0.511</v>
+        <v>-0.513</v>
       </c>
       <c r="O26" s="1">
-        <v>-0.462</v>
+        <v>-0.464</v>
       </c>
       <c r="P26" s="1">
-        <v>-0.392</v>
+        <v>-0.394</v>
       </c>
       <c r="Q26" s="1">
-        <v>-0.304</v>
+        <v>-0.305</v>
       </c>
       <c r="R26" s="1">
-        <v>-0.194</v>
+        <v>-0.195</v>
       </c>
       <c r="S26" s="1">
-        <v>-0.07099999999999999</v>
+        <v>-0.07199999999999999</v>
       </c>
       <c r="T26" s="1">
         <v>0.033</v>
       </c>
       <c r="U26" s="1">
-        <v>0.097</v>
+        <v>0.096</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -2179,64 +2182,64 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>-0.414</v>
+        <v>-0.407</v>
       </c>
       <c r="C27" s="1">
-        <v>-0.356</v>
+        <v>-0.349</v>
       </c>
       <c r="D27" s="1">
-        <v>-0.325</v>
+        <v>-0.321</v>
       </c>
       <c r="E27" s="1">
         <v>-0.373</v>
       </c>
       <c r="F27" s="1">
+        <v>-0.453</v>
+      </c>
+      <c r="G27" s="1">
+        <v>-0.499</v>
+      </c>
+      <c r="H27" s="1">
+        <v>-0.479</v>
+      </c>
+      <c r="I27" s="1">
+        <v>-0.436</v>
+      </c>
+      <c r="J27" s="1">
+        <v>-0.425</v>
+      </c>
+      <c r="K27" s="1">
         <v>-0.449</v>
       </c>
-      <c r="G27" s="1">
-        <v>-0.492</v>
-      </c>
-      <c r="H27" s="1">
-        <v>-0.471</v>
-      </c>
-      <c r="I27" s="1">
-        <v>-0.428</v>
-      </c>
-      <c r="J27" s="1">
-        <v>-0.416</v>
-      </c>
-      <c r="K27" s="1">
-        <v>-0.438</v>
-      </c>
       <c r="L27" s="1">
-        <v>-0.455</v>
+        <v>-0.468</v>
       </c>
       <c r="M27" s="1">
-        <v>-0.434</v>
+        <v>-0.448</v>
       </c>
       <c r="N27" s="1">
-        <v>-0.381</v>
+        <v>-0.393</v>
       </c>
       <c r="O27" s="1">
-        <v>-0.317</v>
+        <v>-0.327</v>
       </c>
       <c r="P27" s="1">
-        <v>-0.246</v>
+        <v>-0.254</v>
       </c>
       <c r="Q27" s="1">
-        <v>-0.162</v>
+        <v>-0.168</v>
       </c>
       <c r="R27" s="1">
-        <v>-0.06900000000000001</v>
+        <v>-0.074</v>
       </c>
       <c r="S27" s="1">
-        <v>0.011</v>
+        <v>0.007</v>
       </c>
       <c r="T27" s="1">
-        <v>0.061</v>
+        <v>0.058</v>
       </c>
       <c r="U27" s="1">
-        <v>0.092</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -2247,61 +2250,126 @@
         <v>0.074</v>
       </c>
       <c r="C28" s="1">
-        <v>0.032</v>
+        <v>0.029</v>
       </c>
       <c r="D28" s="1">
-        <v>-0.066</v>
+        <v>-0.075</v>
       </c>
       <c r="E28" s="1">
-        <v>-0.179</v>
+        <v>-0.198</v>
       </c>
       <c r="F28" s="1">
-        <v>-0.259</v>
+        <v>-0.287</v>
       </c>
       <c r="G28" s="1">
-        <v>-0.278</v>
+        <v>-0.309</v>
       </c>
       <c r="H28" s="1">
-        <v>-0.27</v>
+        <v>-0.301</v>
       </c>
       <c r="I28" s="1">
-        <v>-0.278</v>
+        <v>-0.311</v>
       </c>
       <c r="J28" s="1">
-        <v>-0.307</v>
+        <v>-0.345</v>
       </c>
       <c r="K28" s="1">
-        <v>-0.329</v>
+        <v>-0.373</v>
       </c>
       <c r="L28" s="1">
-        <v>-0.318</v>
+        <v>-0.363</v>
       </c>
       <c r="M28" s="1">
-        <v>-0.279</v>
+        <v>-0.32</v>
       </c>
       <c r="N28" s="1">
-        <v>-0.233</v>
+        <v>-0.267</v>
       </c>
       <c r="O28" s="1">
-        <v>-0.189</v>
+        <v>-0.216</v>
       </c>
       <c r="P28" s="1">
-        <v>-0.145</v>
+        <v>-0.166</v>
       </c>
       <c r="Q28" s="1">
-        <v>-0.101</v>
+        <v>-0.116</v>
       </c>
       <c r="R28" s="1">
-        <v>-0.064</v>
+        <v>-0.073</v>
       </c>
       <c r="S28" s="1">
-        <v>-0.039</v>
+        <v>-0.043</v>
       </c>
       <c r="T28" s="1">
-        <v>-0.022</v>
+        <v>-0.024</v>
       </c>
       <c r="U28" s="1">
         <v>-0.008</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>-0.127</v>
+      </c>
+      <c r="C29" s="1">
+        <v>-0.169</v>
+      </c>
+      <c r="D29" s="1">
+        <v>-0.239</v>
+      </c>
+      <c r="E29" s="1">
+        <v>-0.268</v>
+      </c>
+      <c r="F29" s="1">
+        <v>-0.239</v>
+      </c>
+      <c r="G29" s="1">
+        <v>-0.199</v>
+      </c>
+      <c r="H29" s="1">
+        <v>-0.182</v>
+      </c>
+      <c r="I29" s="1">
+        <v>-0.178</v>
+      </c>
+      <c r="J29" s="1">
+        <v>-0.165</v>
+      </c>
+      <c r="K29" s="1">
+        <v>-0.136</v>
+      </c>
+      <c r="L29" s="1">
+        <v>-0.105</v>
+      </c>
+      <c r="M29" s="1">
+        <v>-0.082</v>
+      </c>
+      <c r="N29" s="1">
+        <v>-0.064</v>
+      </c>
+      <c r="O29" s="1">
+        <v>-0.041</v>
+      </c>
+      <c r="P29" s="1">
+        <v>-0.014</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0.011</v>
+      </c>
+      <c r="R29" s="1">
+        <v>0.027</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0.036</v>
+      </c>
+      <c r="T29" s="1">
+        <v>0.048</v>
+      </c>
+      <c r="U29" s="1">
+        <v>0.065</v>
       </c>
     </row>
   </sheetData>
@@ -2319,22 +2387,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: XRO fcst update
</commit_message>
<xml_diff>
--- a/content/climate/XRO/XRO_ENSO_fcst.xlsx
+++ b/content/climate/XRO/XRO_ENSO_fcst.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>init</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>2025-04</t>
+  </si>
+  <si>
+    <t>2025-05</t>
   </si>
   <si>
     <t>Readme</t>
@@ -478,7 +481,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,7 +492,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2">
         <v>0</v>
@@ -560,61 +563,61 @@
         <v>-0.68</v>
       </c>
       <c r="C2" s="1">
-        <v>-0.666</v>
+        <v>-0.731</v>
       </c>
       <c r="D2" s="1">
-        <v>-0.584</v>
+        <v>-0.711</v>
       </c>
       <c r="E2" s="1">
-        <v>-0.392</v>
+        <v>-0.51</v>
       </c>
       <c r="F2" s="1">
-        <v>-0.092</v>
+        <v>-0.147</v>
       </c>
       <c r="G2" s="1">
-        <v>0.257</v>
+        <v>0.261</v>
       </c>
       <c r="H2" s="1">
-        <v>0.5629999999999999</v>
+        <v>0.573</v>
       </c>
       <c r="I2" s="1">
-        <v>0.778</v>
+        <v>0.771</v>
       </c>
       <c r="J2" s="1">
-        <v>0.949</v>
+        <v>0.954</v>
       </c>
       <c r="K2" s="1">
-        <v>1.152</v>
+        <v>1.232</v>
       </c>
       <c r="L2" s="1">
-        <v>1.396</v>
+        <v>1.59</v>
       </c>
       <c r="M2" s="1">
-        <v>1.589</v>
+        <v>1.858</v>
       </c>
       <c r="N2" s="1">
-        <v>1.638</v>
+        <v>1.913</v>
       </c>
       <c r="O2" s="1">
-        <v>1.527</v>
+        <v>1.781</v>
       </c>
       <c r="P2" s="1">
-        <v>1.29</v>
+        <v>1.53</v>
       </c>
       <c r="Q2" s="1">
-        <v>0.979</v>
+        <v>1.222</v>
       </c>
       <c r="R2" s="1">
-        <v>0.657</v>
+        <v>0.899</v>
       </c>
       <c r="S2" s="1">
-        <v>0.361</v>
+        <v>0.602</v>
       </c>
       <c r="T2" s="1">
-        <v>0.123</v>
+        <v>0.362</v>
       </c>
       <c r="U2" s="1">
-        <v>-0.031</v>
+        <v>0.185</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -622,64 +625,64 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>-0.46</v>
+        <v>-0.473</v>
       </c>
       <c r="C3" s="1">
-        <v>-0.4</v>
+        <v>-0.459</v>
       </c>
       <c r="D3" s="1">
-        <v>-0.226</v>
+        <v>-0.313</v>
       </c>
       <c r="E3" s="1">
-        <v>0.041</v>
+        <v>-0.021</v>
       </c>
       <c r="F3" s="1">
-        <v>0.342</v>
+        <v>0.296</v>
       </c>
       <c r="G3" s="1">
+        <v>0.529</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.671</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.794</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.972</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1.194</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1.351</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1.361</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1.238</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1.048</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0.833</v>
+      </c>
+      <c r="Q3" s="1">
         <v>0.605</v>
       </c>
-      <c r="H3" s="1">
-        <v>0.796</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.951</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1.131</v>
-      </c>
-      <c r="K3" s="1">
-        <v>1.334</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1.479</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1.491</v>
-      </c>
-      <c r="N3" s="1">
-        <v>1.372</v>
-      </c>
-      <c r="O3" s="1">
-        <v>1.152</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0.869</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0.5669999999999999</v>
-      </c>
       <c r="R3" s="1">
-        <v>0.278</v>
+        <v>0.379</v>
       </c>
       <c r="S3" s="1">
-        <v>0.042</v>
+        <v>0.188</v>
       </c>
       <c r="T3" s="1">
-        <v>-0.107</v>
+        <v>0.047</v>
       </c>
       <c r="U3" s="1">
-        <v>-0.193</v>
+        <v>-0.048</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -687,64 +690,64 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>-0.003</v>
+        <v>-0.02</v>
       </c>
       <c r="C4" s="1">
-        <v>0.056</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D4" s="1">
-        <v>0.2</v>
+        <v>0.277</v>
       </c>
       <c r="E4" s="1">
-        <v>0.385</v>
+        <v>0.485</v>
       </c>
       <c r="F4" s="1">
-        <v>0.551</v>
+        <v>0.613</v>
       </c>
       <c r="G4" s="1">
-        <v>0.67</v>
+        <v>0.671</v>
       </c>
       <c r="H4" s="1">
-        <v>0.766</v>
+        <v>0.728</v>
       </c>
       <c r="I4" s="1">
-        <v>0.88</v>
+        <v>0.84</v>
       </c>
       <c r="J4" s="1">
-        <v>1.012</v>
+        <v>0.989</v>
       </c>
       <c r="K4" s="1">
-        <v>1.105</v>
+        <v>1.091</v>
       </c>
       <c r="L4" s="1">
-        <v>1.102</v>
+        <v>1.075</v>
       </c>
       <c r="M4" s="1">
-        <v>0.999</v>
+        <v>0.955</v>
       </c>
       <c r="N4" s="1">
-        <v>0.825</v>
+        <v>0.798</v>
       </c>
       <c r="O4" s="1">
-        <v>0.612</v>
+        <v>0.635</v>
       </c>
       <c r="P4" s="1">
-        <v>0.38</v>
+        <v>0.454</v>
       </c>
       <c r="Q4" s="1">
-        <v>0.148</v>
+        <v>0.258</v>
       </c>
       <c r="R4" s="1">
-        <v>-0.047</v>
+        <v>0.08</v>
       </c>
       <c r="S4" s="1">
-        <v>-0.17</v>
+        <v>-0.055</v>
       </c>
       <c r="T4" s="1">
-        <v>-0.24</v>
+        <v>-0.145</v>
       </c>
       <c r="U4" s="1">
-        <v>-0.309</v>
+        <v>-0.219</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -752,64 +755,64 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>0.117</v>
+        <v>0.182</v>
       </c>
       <c r="C5" s="1">
-        <v>0.213</v>
+        <v>0.333</v>
       </c>
       <c r="D5" s="1">
-        <v>0.406</v>
+        <v>0.57</v>
       </c>
       <c r="E5" s="1">
-        <v>0.625</v>
+        <v>0.742</v>
       </c>
       <c r="F5" s="1">
-        <v>0.827</v>
+        <v>0.846</v>
       </c>
       <c r="G5" s="1">
-        <v>0.99</v>
+        <v>0.9320000000000001</v>
       </c>
       <c r="H5" s="1">
-        <v>1.132</v>
+        <v>1.056</v>
       </c>
       <c r="I5" s="1">
-        <v>1.257</v>
+        <v>1.205</v>
       </c>
       <c r="J5" s="1">
-        <v>1.321</v>
+        <v>1.287</v>
       </c>
       <c r="K5" s="1">
-        <v>1.288</v>
+        <v>1.232</v>
       </c>
       <c r="L5" s="1">
-        <v>1.161</v>
+        <v>1.071</v>
       </c>
       <c r="M5" s="1">
-        <v>0.958</v>
+        <v>0.888</v>
       </c>
       <c r="N5" s="1">
-        <v>0.695</v>
+        <v>0.707</v>
       </c>
       <c r="O5" s="1">
-        <v>0.396</v>
+        <v>0.496</v>
       </c>
       <c r="P5" s="1">
-        <v>0.09</v>
+        <v>0.254</v>
       </c>
       <c r="Q5" s="1">
-        <v>-0.168</v>
+        <v>0.025</v>
       </c>
       <c r="R5" s="1">
-        <v>-0.322</v>
+        <v>-0.153</v>
       </c>
       <c r="S5" s="1">
-        <v>-0.399</v>
+        <v>-0.27</v>
       </c>
       <c r="T5" s="1">
-        <v>-0.484</v>
+        <v>-0.364</v>
       </c>
       <c r="U5" s="1">
-        <v>-0.612</v>
+        <v>-0.464</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -817,64 +820,64 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>0.475</v>
+        <v>0.464</v>
       </c>
       <c r="C6" s="1">
-        <v>0.616</v>
+        <v>0.626</v>
       </c>
       <c r="D6" s="1">
-        <v>0.847</v>
+        <v>0.843</v>
       </c>
       <c r="E6" s="1">
-        <v>1.052</v>
+        <v>0.969</v>
       </c>
       <c r="F6" s="1">
-        <v>1.219</v>
+        <v>1.063</v>
       </c>
       <c r="G6" s="1">
-        <v>1.361</v>
+        <v>1.193</v>
       </c>
       <c r="H6" s="1">
-        <v>1.472</v>
+        <v>1.341</v>
       </c>
       <c r="I6" s="1">
-        <v>1.506</v>
+        <v>1.406</v>
       </c>
       <c r="J6" s="1">
-        <v>1.437</v>
+        <v>1.322</v>
       </c>
       <c r="K6" s="1">
-        <v>1.282</v>
+        <v>1.131</v>
       </c>
       <c r="L6" s="1">
-        <v>1.052</v>
+        <v>0.927</v>
       </c>
       <c r="M6" s="1">
-        <v>0.756</v>
+        <v>0.735</v>
       </c>
       <c r="N6" s="1">
-        <v>0.415</v>
+        <v>0.507</v>
       </c>
       <c r="O6" s="1">
-        <v>0.062</v>
+        <v>0.244</v>
       </c>
       <c r="P6" s="1">
-        <v>-0.235</v>
+        <v>-0.008</v>
       </c>
       <c r="Q6" s="1">
-        <v>-0.408</v>
+        <v>-0.202</v>
       </c>
       <c r="R6" s="1">
-        <v>-0.491</v>
+        <v>-0.328</v>
       </c>
       <c r="S6" s="1">
-        <v>-0.584</v>
+        <v>-0.43</v>
       </c>
       <c r="T6" s="1">
-        <v>-0.731</v>
+        <v>-0.542</v>
       </c>
       <c r="U6" s="1">
-        <v>-0.877</v>
+        <v>-0.646</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -882,64 +885,64 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>0.853</v>
+        <v>0.904</v>
       </c>
       <c r="C7" s="1">
-        <v>0.99</v>
+        <v>1.009</v>
       </c>
       <c r="D7" s="1">
-        <v>1.209</v>
+        <v>1.135</v>
       </c>
       <c r="E7" s="1">
-        <v>1.4</v>
+        <v>1.233</v>
       </c>
       <c r="F7" s="1">
-        <v>1.557</v>
+        <v>1.358</v>
       </c>
       <c r="G7" s="1">
-        <v>1.654</v>
+        <v>1.477</v>
       </c>
       <c r="H7" s="1">
-        <v>1.645</v>
+        <v>1.498</v>
       </c>
       <c r="I7" s="1">
-        <v>1.532</v>
+        <v>1.374</v>
       </c>
       <c r="J7" s="1">
-        <v>1.344</v>
+        <v>1.158</v>
       </c>
       <c r="K7" s="1">
-        <v>1.089</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="L7" s="1">
-        <v>0.762</v>
+        <v>0.729</v>
       </c>
       <c r="M7" s="1">
-        <v>0.375</v>
+        <v>0.464</v>
       </c>
       <c r="N7" s="1">
-        <v>-0.038</v>
+        <v>0.153</v>
       </c>
       <c r="O7" s="1">
-        <v>-0.386</v>
+        <v>-0.141</v>
       </c>
       <c r="P7" s="1">
-        <v>-0.578</v>
+        <v>-0.356</v>
       </c>
       <c r="Q7" s="1">
-        <v>-0.658</v>
+        <v>-0.483</v>
       </c>
       <c r="R7" s="1">
-        <v>-0.757</v>
+        <v>-0.588</v>
       </c>
       <c r="S7" s="1">
-        <v>-0.931</v>
+        <v>-0.72</v>
       </c>
       <c r="T7" s="1">
-        <v>-1.108</v>
+        <v>-0.851</v>
       </c>
       <c r="U7" s="1">
-        <v>-1.149</v>
+        <v>-0.906</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -947,64 +950,64 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>1.021</v>
+        <v>1.051</v>
       </c>
       <c r="C8" s="1">
-        <v>1.175</v>
+        <v>1.166</v>
       </c>
       <c r="D8" s="1">
-        <v>1.415</v>
+        <v>1.338</v>
       </c>
       <c r="E8" s="1">
-        <v>1.604</v>
+        <v>1.494</v>
       </c>
       <c r="F8" s="1">
-        <v>1.719</v>
+        <v>1.59</v>
       </c>
       <c r="G8" s="1">
-        <v>1.713</v>
+        <v>1.551</v>
       </c>
       <c r="H8" s="1">
-        <v>1.593</v>
+        <v>1.365</v>
       </c>
       <c r="I8" s="1">
-        <v>1.395</v>
+        <v>1.111</v>
       </c>
       <c r="J8" s="1">
-        <v>1.129</v>
+        <v>0.884</v>
       </c>
       <c r="K8" s="1">
-        <v>0.794</v>
+        <v>0.67</v>
       </c>
       <c r="L8" s="1">
-        <v>0.4</v>
+        <v>0.392</v>
       </c>
       <c r="M8" s="1">
-        <v>-0.019</v>
+        <v>0.056</v>
       </c>
       <c r="N8" s="1">
-        <v>-0.372</v>
+        <v>-0.262</v>
       </c>
       <c r="O8" s="1">
-        <v>-0.5679999999999999</v>
+        <v>-0.484</v>
       </c>
       <c r="P8" s="1">
-        <v>-0.65</v>
+        <v>-0.604</v>
       </c>
       <c r="Q8" s="1">
-        <v>-0.752</v>
+        <v>-0.709</v>
       </c>
       <c r="R8" s="1">
-        <v>-0.929</v>
+        <v>-0.858</v>
       </c>
       <c r="S8" s="1">
-        <v>-1.109</v>
+        <v>-1.014</v>
       </c>
       <c r="T8" s="1">
-        <v>-1.152</v>
+        <v>-1.08</v>
       </c>
       <c r="U8" s="1">
-        <v>-1.031</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1012,64 +1015,64 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>1.348</v>
+        <v>1.304</v>
       </c>
       <c r="C9" s="1">
-        <v>1.517</v>
+        <v>1.449</v>
       </c>
       <c r="D9" s="1">
-        <v>1.788</v>
+        <v>1.667</v>
       </c>
       <c r="E9" s="1">
-        <v>1.951</v>
+        <v>1.771</v>
       </c>
       <c r="F9" s="1">
-        <v>1.95</v>
+        <v>1.699</v>
       </c>
       <c r="G9" s="1">
-        <v>1.816</v>
+        <v>1.479</v>
       </c>
       <c r="H9" s="1">
-        <v>1.601</v>
+        <v>1.209</v>
       </c>
       <c r="I9" s="1">
-        <v>1.305</v>
+        <v>0.969</v>
       </c>
       <c r="J9" s="1">
-        <v>0.914</v>
+        <v>0.725</v>
       </c>
       <c r="K9" s="1">
-        <v>0.448</v>
+        <v>0.399</v>
       </c>
       <c r="L9" s="1">
-        <v>-0.045</v>
+        <v>0.01</v>
       </c>
       <c r="M9" s="1">
-        <v>-0.456</v>
+        <v>-0.349</v>
       </c>
       <c r="N9" s="1">
-        <v>-0.673</v>
+        <v>-0.589</v>
       </c>
       <c r="O9" s="1">
-        <v>-0.756</v>
+        <v>-0.708</v>
       </c>
       <c r="P9" s="1">
-        <v>-0.863</v>
+        <v>-0.8129999999999999</v>
       </c>
       <c r="Q9" s="1">
-        <v>-1.059</v>
+        <v>-0.977</v>
       </c>
       <c r="R9" s="1">
-        <v>-1.259</v>
+        <v>-1.155</v>
       </c>
       <c r="S9" s="1">
-        <v>-1.3</v>
+        <v>-1.228</v>
       </c>
       <c r="T9" s="1">
-        <v>-1.156</v>
+        <v>-1.133</v>
       </c>
       <c r="U9" s="1">
-        <v>-0.959</v>
+        <v>-0.9429999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1077,64 +1080,64 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>1.598</v>
+        <v>1.555</v>
       </c>
       <c r="C10" s="1">
-        <v>1.76</v>
+        <v>1.699</v>
       </c>
       <c r="D10" s="1">
-        <v>1.968</v>
+        <v>1.864</v>
       </c>
       <c r="E10" s="1">
-        <v>1.988</v>
+        <v>1.832</v>
       </c>
       <c r="F10" s="1">
-        <v>1.851</v>
+        <v>1.623</v>
       </c>
       <c r="G10" s="1">
-        <v>1.624</v>
+        <v>1.345</v>
       </c>
       <c r="H10" s="1">
-        <v>1.312</v>
+        <v>1.086</v>
       </c>
       <c r="I10" s="1">
-        <v>0.907</v>
+        <v>0.823</v>
       </c>
       <c r="J10" s="1">
-        <v>0.429</v>
+        <v>0.486</v>
       </c>
       <c r="K10" s="1">
-        <v>-0.077</v>
+        <v>0.095</v>
       </c>
       <c r="L10" s="1">
-        <v>-0.501</v>
+        <v>-0.265</v>
       </c>
       <c r="M10" s="1">
-        <v>-0.723</v>
+        <v>-0.51</v>
       </c>
       <c r="N10" s="1">
-        <v>-0.805</v>
+        <v>-0.639</v>
       </c>
       <c r="O10" s="1">
-        <v>-0.912</v>
+        <v>-0.748</v>
       </c>
       <c r="P10" s="1">
-        <v>-1.113</v>
+        <v>-0.903</v>
       </c>
       <c r="Q10" s="1">
-        <v>-1.316</v>
+        <v>-1.068</v>
       </c>
       <c r="R10" s="1">
-        <v>-1.355</v>
+        <v>-1.138</v>
       </c>
       <c r="S10" s="1">
-        <v>-1.204</v>
+        <v>-1.05</v>
       </c>
       <c r="T10" s="1">
-        <v>-0.999</v>
+        <v>-0.873</v>
       </c>
       <c r="U10" s="1">
-        <v>-0.847</v>
+        <v>-0.712</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1142,64 +1145,64 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>1.613</v>
+        <v>1.596</v>
       </c>
       <c r="C11" s="1">
-        <v>1.749</v>
+        <v>1.724</v>
       </c>
       <c r="D11" s="1">
-        <v>1.851</v>
+        <v>1.802</v>
       </c>
       <c r="E11" s="1">
-        <v>1.748</v>
+        <v>1.655</v>
       </c>
       <c r="F11" s="1">
-        <v>1.52</v>
+        <v>1.4</v>
       </c>
       <c r="G11" s="1">
-        <v>1.209</v>
+        <v>1.14</v>
       </c>
       <c r="H11" s="1">
-        <v>0.828</v>
+        <v>0.871</v>
       </c>
       <c r="I11" s="1">
-        <v>0.389</v>
+        <v>0.543</v>
       </c>
       <c r="J11" s="1">
-        <v>-0.079</v>
+        <v>0.176</v>
       </c>
       <c r="K11" s="1">
-        <v>-0.475</v>
+        <v>-0.156</v>
       </c>
       <c r="L11" s="1">
-        <v>-0.6879999999999999</v>
+        <v>-0.386</v>
       </c>
       <c r="M11" s="1">
-        <v>-0.77</v>
+        <v>-0.516</v>
       </c>
       <c r="N11" s="1">
+        <v>-0.621</v>
+      </c>
+      <c r="O11" s="1">
+        <v>-0.756</v>
+      </c>
+      <c r="P11" s="1">
+        <v>-0.893</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>-0.948</v>
+      </c>
+      <c r="R11" s="1">
         <v>-0.874</v>
       </c>
-      <c r="O11" s="1">
-        <v>-1.062</v>
-      </c>
-      <c r="P11" s="1">
-        <v>-1.251</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>-1.287</v>
-      </c>
-      <c r="R11" s="1">
-        <v>-1.145</v>
-      </c>
       <c r="S11" s="1">
-        <v>-0.952</v>
+        <v>-0.725</v>
       </c>
       <c r="T11" s="1">
-        <v>-0.802</v>
+        <v>-0.588</v>
       </c>
       <c r="U11" s="1">
-        <v>-0.711</v>
+        <v>-0.495</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1207,64 +1210,64 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>1.811</v>
+        <v>1.889</v>
       </c>
       <c r="C12" s="1">
-        <v>1.801</v>
+        <v>1.845</v>
       </c>
       <c r="D12" s="1">
-        <v>1.684</v>
+        <v>1.671</v>
       </c>
       <c r="E12" s="1">
-        <v>1.464</v>
+        <v>1.423</v>
       </c>
       <c r="F12" s="1">
-        <v>1.156</v>
+        <v>1.164</v>
       </c>
       <c r="G12" s="1">
-        <v>0.764</v>
+        <v>0.867</v>
       </c>
       <c r="H12" s="1">
-        <v>0.3</v>
+        <v>0.491</v>
       </c>
       <c r="I12" s="1">
-        <v>-0.201</v>
+        <v>0.075</v>
       </c>
       <c r="J12" s="1">
-        <v>-0.62</v>
+        <v>-0.294</v>
       </c>
       <c r="K12" s="1">
-        <v>-0.83</v>
+        <v>-0.54</v>
       </c>
       <c r="L12" s="1">
-        <v>-0.899</v>
+        <v>-0.669</v>
       </c>
       <c r="M12" s="1">
-        <v>-1.006</v>
+        <v>-0.779</v>
       </c>
       <c r="N12" s="1">
-        <v>-1.217</v>
+        <v>-0.9350000000000001</v>
       </c>
       <c r="O12" s="1">
-        <v>-1.432</v>
+        <v>-1.099</v>
       </c>
       <c r="P12" s="1">
-        <v>-1.469</v>
+        <v>-1.164</v>
       </c>
       <c r="Q12" s="1">
-        <v>-1.305</v>
+        <v>-1.07</v>
       </c>
       <c r="R12" s="1">
-        <v>-1.085</v>
+        <v>-0.888</v>
       </c>
       <c r="S12" s="1">
-        <v>-0.918</v>
+        <v>-0.723</v>
       </c>
       <c r="T12" s="1">
-        <v>-0.821</v>
+        <v>-0.609</v>
       </c>
       <c r="U12" s="1">
-        <v>-0.755</v>
+        <v>-0.532</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1272,64 +1275,64 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>1.974</v>
+        <v>1.975</v>
       </c>
       <c r="C13" s="1">
-        <v>1.925</v>
+        <v>1.86</v>
       </c>
       <c r="D13" s="1">
-        <v>1.725</v>
+        <v>1.594</v>
       </c>
       <c r="E13" s="1">
-        <v>1.376</v>
+        <v>1.298</v>
       </c>
       <c r="F13" s="1">
-        <v>0.91</v>
+        <v>0.958</v>
       </c>
       <c r="G13" s="1">
-        <v>0.377</v>
+        <v>0.534</v>
       </c>
       <c r="H13" s="1">
-        <v>-0.18</v>
+        <v>0.065</v>
       </c>
       <c r="I13" s="1">
-        <v>-0.644</v>
+        <v>-0.358</v>
       </c>
       <c r="J13" s="1">
-        <v>-0.88</v>
+        <v>-0.647</v>
       </c>
       <c r="K13" s="1">
-        <v>-0.96</v>
+        <v>-0.8</v>
       </c>
       <c r="L13" s="1">
-        <v>-1.08</v>
+        <v>-0.924</v>
       </c>
       <c r="M13" s="1">
-        <v>-1.308</v>
+        <v>-1.098</v>
       </c>
       <c r="N13" s="1">
-        <v>-1.535</v>
+        <v>-1.283</v>
       </c>
       <c r="O13" s="1">
-        <v>-1.568</v>
+        <v>-1.361</v>
       </c>
       <c r="P13" s="1">
-        <v>-1.388</v>
+        <v>-1.257</v>
       </c>
       <c r="Q13" s="1">
-        <v>-1.157</v>
+        <v>-1.048</v>
       </c>
       <c r="R13" s="1">
-        <v>-0.989</v>
+        <v>-0.853</v>
       </c>
       <c r="S13" s="1">
-        <v>-0.902</v>
+        <v>-0.711</v>
       </c>
       <c r="T13" s="1">
-        <v>-0.852</v>
+        <v>-0.613</v>
       </c>
       <c r="U13" s="1">
-        <v>-0.785</v>
+        <v>-0.547</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1337,64 +1340,64 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>1.805</v>
+        <v>1.78</v>
       </c>
       <c r="C14" s="1">
-        <v>1.714</v>
+        <v>1.668</v>
       </c>
       <c r="D14" s="1">
-        <v>1.401</v>
+        <v>1.389</v>
       </c>
       <c r="E14" s="1">
-        <v>0.928</v>
+        <v>0.989</v>
       </c>
       <c r="F14" s="1">
-        <v>0.401</v>
+        <v>0.471</v>
       </c>
       <c r="G14" s="1">
-        <v>-0.126</v>
+        <v>-0.089</v>
       </c>
       <c r="H14" s="1">
-        <v>-0.5620000000000001</v>
+        <v>-0.573</v>
       </c>
       <c r="I14" s="1">
-        <v>-0.793</v>
+        <v>-0.869</v>
       </c>
       <c r="J14" s="1">
-        <v>-0.879</v>
+        <v>-0.987</v>
       </c>
       <c r="K14" s="1">
-        <v>-0.997</v>
+        <v>-1.087</v>
       </c>
       <c r="L14" s="1">
-        <v>-1.211</v>
+        <v>-1.27</v>
       </c>
       <c r="M14" s="1">
-        <v>-1.418</v>
+        <v>-1.48</v>
       </c>
       <c r="N14" s="1">
-        <v>-1.446</v>
+        <v>-1.56</v>
       </c>
       <c r="O14" s="1">
-        <v>-1.282</v>
+        <v>-1.421</v>
       </c>
       <c r="P14" s="1">
-        <v>-1.072</v>
+        <v>-1.172</v>
       </c>
       <c r="Q14" s="1">
-        <v>-0.916</v>
+        <v>-0.959</v>
       </c>
       <c r="R14" s="1">
-        <v>-0.831</v>
+        <v>-0.823</v>
       </c>
       <c r="S14" s="1">
-        <v>-0.78</v>
+        <v>-0.736</v>
       </c>
       <c r="T14" s="1">
-        <v>-0.716</v>
+        <v>-0.673</v>
       </c>
       <c r="U14" s="1">
-        <v>-0.631</v>
+        <v>-0.618</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1402,64 +1405,64 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>1.592</v>
+        <v>1.537</v>
       </c>
       <c r="C15" s="1">
-        <v>1.373</v>
+        <v>1.359</v>
       </c>
       <c r="D15" s="1">
-        <v>0.918</v>
+        <v>0.986</v>
       </c>
       <c r="E15" s="1">
-        <v>0.406</v>
+        <v>0.496</v>
       </c>
       <c r="F15" s="1">
-        <v>-0.116</v>
+        <v>-0.063</v>
       </c>
       <c r="G15" s="1">
-        <v>-0.556</v>
+        <v>-0.571</v>
       </c>
       <c r="H15" s="1">
-        <v>-0.792</v>
+        <v>-0.897</v>
       </c>
       <c r="I15" s="1">
-        <v>-0.877</v>
+        <v>-1.032</v>
       </c>
       <c r="J15" s="1">
-        <v>-0.99</v>
+        <v>-1.138</v>
       </c>
       <c r="K15" s="1">
-        <v>-1.196</v>
+        <v>-1.331</v>
       </c>
       <c r="L15" s="1">
-        <v>-1.393</v>
+        <v>-1.555</v>
       </c>
       <c r="M15" s="1">
-        <v>-1.416</v>
+        <v>-1.65</v>
       </c>
       <c r="N15" s="1">
+        <v>-1.515</v>
+      </c>
+      <c r="O15" s="1">
         <v>-1.256</v>
       </c>
-      <c r="O15" s="1">
-        <v>-1.054</v>
-      </c>
       <c r="P15" s="1">
-        <v>-0.904</v>
+        <v>-1.028</v>
       </c>
       <c r="Q15" s="1">
-        <v>-0.822</v>
+        <v>-0.882</v>
       </c>
       <c r="R15" s="1">
-        <v>-0.774</v>
+        <v>-0.795</v>
       </c>
       <c r="S15" s="1">
-        <v>-0.715</v>
+        <v>-0.737</v>
       </c>
       <c r="T15" s="1">
-        <v>-0.633</v>
+        <v>-0.6899999999999999</v>
       </c>
       <c r="U15" s="1">
-        <v>-0.5580000000000001</v>
+        <v>-0.65</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1467,64 +1470,64 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>1.299</v>
+        <v>1.227</v>
       </c>
       <c r="C16" s="1">
-        <v>1.006</v>
+        <v>0.996</v>
       </c>
       <c r="D16" s="1">
-        <v>0.471</v>
+        <v>0.533</v>
       </c>
       <c r="E16" s="1">
-        <v>-0.074</v>
+        <v>0.015</v>
       </c>
       <c r="F16" s="1">
-        <v>-0.519</v>
+        <v>-0.458</v>
       </c>
       <c r="G16" s="1">
-        <v>-0.744</v>
+        <v>-0.771</v>
       </c>
       <c r="H16" s="1">
-        <v>-0.822</v>
+        <v>-0.909</v>
       </c>
       <c r="I16" s="1">
-        <v>-0.93</v>
+        <v>-1.011</v>
       </c>
       <c r="J16" s="1">
-        <v>-1.129</v>
+        <v>-1.181</v>
       </c>
       <c r="K16" s="1">
-        <v>-1.319</v>
+        <v>-1.381</v>
       </c>
       <c r="L16" s="1">
-        <v>-1.342</v>
+        <v>-1.475</v>
       </c>
       <c r="M16" s="1">
-        <v>-1.189</v>
+        <v>-1.368</v>
       </c>
       <c r="N16" s="1">
-        <v>-0.997</v>
+        <v>-1.139</v>
       </c>
       <c r="O16" s="1">
-        <v>-0.861</v>
+        <v>-0.927</v>
       </c>
       <c r="P16" s="1">
-        <v>-0.798</v>
+        <v>-0.783</v>
       </c>
       <c r="Q16" s="1">
-        <v>-0.772</v>
+        <v>-0.694</v>
       </c>
       <c r="R16" s="1">
-        <v>-0.732</v>
+        <v>-0.639</v>
       </c>
       <c r="S16" s="1">
-        <v>-0.659</v>
+        <v>-0.6</v>
       </c>
       <c r="T16" s="1">
-        <v>-0.588</v>
+        <v>-0.571</v>
       </c>
       <c r="U16" s="1">
-        <v>-0.5639999999999999</v>
+        <v>-0.5669999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -1532,64 +1535,64 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>0.895</v>
+        <v>0.847</v>
       </c>
       <c r="C17" s="1">
-        <v>0.6</v>
+        <v>0.571</v>
       </c>
       <c r="D17" s="1">
-        <v>0.083</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="E17" s="1">
-        <v>-0.339</v>
+        <v>-0.391</v>
       </c>
       <c r="F17" s="1">
-        <v>-0.5590000000000001</v>
+        <v>-0.704</v>
       </c>
       <c r="G17" s="1">
-        <v>-0.645</v>
+        <v>-0.854</v>
       </c>
       <c r="H17" s="1">
-        <v>-0.751</v>
+        <v>-0.967</v>
       </c>
       <c r="I17" s="1">
-        <v>-0.925</v>
+        <v>-1.138</v>
       </c>
       <c r="J17" s="1">
-        <v>-1.087</v>
+        <v>-1.334</v>
       </c>
       <c r="K17" s="1">
+        <v>-1.428</v>
+      </c>
+      <c r="L17" s="1">
+        <v>-1.328</v>
+      </c>
+      <c r="M17" s="1">
         <v>-1.108</v>
       </c>
-      <c r="L17" s="1">
-        <v>-0.98</v>
-      </c>
-      <c r="M17" s="1">
-        <v>-0.822</v>
-      </c>
       <c r="N17" s="1">
-        <v>-0.714</v>
+        <v>-0.898</v>
       </c>
       <c r="O17" s="1">
-        <v>-0.672</v>
+        <v>-0.75</v>
       </c>
       <c r="P17" s="1">
-        <v>-0.666</v>
+        <v>-0.658</v>
       </c>
       <c r="Q17" s="1">
-        <v>-0.648</v>
+        <v>-0.605</v>
       </c>
       <c r="R17" s="1">
-        <v>-0.597</v>
+        <v>-0.574</v>
       </c>
       <c r="S17" s="1">
-        <v>-0.54</v>
+        <v>-0.55</v>
       </c>
       <c r="T17" s="1">
-        <v>-0.524</v>
+        <v>-0.549</v>
       </c>
       <c r="U17" s="1">
-        <v>-0.5590000000000001</v>
+        <v>-0.574</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -1597,64 +1600,64 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>0.293</v>
+        <v>0.315</v>
       </c>
       <c r="C18" s="1">
-        <v>0.006</v>
+        <v>0.008</v>
       </c>
       <c r="D18" s="1">
-        <v>-0.412</v>
+        <v>-0.472</v>
       </c>
       <c r="E18" s="1">
-        <v>-0.621</v>
+        <v>-0.792</v>
       </c>
       <c r="F18" s="1">
-        <v>-0.704</v>
+        <v>-0.9409999999999999</v>
       </c>
       <c r="G18" s="1">
-        <v>-0.819</v>
+        <v>-1.049</v>
       </c>
       <c r="H18" s="1">
-        <v>-0.999</v>
+        <v>-1.213</v>
       </c>
       <c r="I18" s="1">
-        <v>-1.152</v>
+        <v>-1.396</v>
       </c>
       <c r="J18" s="1">
-        <v>-1.153</v>
+        <v>-1.476</v>
       </c>
       <c r="K18" s="1">
-        <v>-1.014</v>
+        <v>-1.37</v>
       </c>
       <c r="L18" s="1">
-        <v>-0.853</v>
+        <v>-1.151</v>
       </c>
       <c r="M18" s="1">
-        <v>-0.742</v>
+        <v>-0.9360000000000001</v>
       </c>
       <c r="N18" s="1">
-        <v>-0.6889999999999999</v>
+        <v>-0.769</v>
       </c>
       <c r="O18" s="1">
-        <v>-0.667</v>
+        <v>-0.645</v>
       </c>
       <c r="P18" s="1">
-        <v>-0.636</v>
+        <v>-0.5629999999999999</v>
       </c>
       <c r="Q18" s="1">
-        <v>-0.58</v>
+        <v>-0.514</v>
       </c>
       <c r="R18" s="1">
-        <v>-0.523</v>
+        <v>-0.483</v>
       </c>
       <c r="S18" s="1">
-        <v>-0.506</v>
+        <v>-0.472</v>
       </c>
       <c r="T18" s="1">
-        <v>-0.536</v>
+        <v>-0.479</v>
       </c>
       <c r="U18" s="1">
-        <v>-0.573</v>
+        <v>-0.478</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -1662,64 +1665,64 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>0.266</v>
+        <v>0.252</v>
       </c>
       <c r="C19" s="1">
-        <v>0.07000000000000001</v>
+        <v>0.023</v>
       </c>
       <c r="D19" s="1">
-        <v>-0.181</v>
+        <v>-0.304</v>
       </c>
       <c r="E19" s="1">
-        <v>-0.323</v>
+        <v>-0.501</v>
       </c>
       <c r="F19" s="1">
-        <v>-0.472</v>
+        <v>-0.655</v>
       </c>
       <c r="G19" s="1">
-        <v>-0.65</v>
+        <v>-0.831</v>
       </c>
       <c r="H19" s="1">
-        <v>-0.786</v>
+        <v>-1.001</v>
       </c>
       <c r="I19" s="1">
-        <v>-0.798</v>
+        <v>-1.076</v>
       </c>
       <c r="J19" s="1">
-        <v>-0.703</v>
+        <v>-0.997</v>
       </c>
       <c r="K19" s="1">
-        <v>-0.597</v>
+        <v>-0.822</v>
       </c>
       <c r="L19" s="1">
-        <v>-0.541</v>
+        <v>-0.663</v>
       </c>
       <c r="M19" s="1">
-        <v>-0.548</v>
+        <v>-0.576</v>
       </c>
       <c r="N19" s="1">
-        <v>-0.594</v>
+        <v>-0.553</v>
       </c>
       <c r="O19" s="1">
-        <v>-0.626</v>
+        <v>-0.5610000000000001</v>
       </c>
       <c r="P19" s="1">
-        <v>-0.609</v>
+        <v>-0.5659999999999999</v>
       </c>
       <c r="Q19" s="1">
-        <v>-0.573</v>
+        <v>-0.5610000000000001</v>
       </c>
       <c r="R19" s="1">
         <v>-0.575</v>
       </c>
       <c r="S19" s="1">
-        <v>-0.635</v>
+        <v>-0.622</v>
       </c>
       <c r="T19" s="1">
-        <v>-0.704</v>
+        <v>-0.666</v>
       </c>
       <c r="U19" s="1">
-        <v>-0.714</v>
+        <v>-0.672</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -1727,64 +1730,64 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>0.101</v>
+        <v>0.192</v>
       </c>
       <c r="C20" s="1">
-        <v>0.017</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D20" s="1">
-        <v>-0.111</v>
+        <v>-0.118</v>
       </c>
       <c r="E20" s="1">
-        <v>-0.253</v>
+        <v>-0.289</v>
       </c>
       <c r="F20" s="1">
-        <v>-0.401</v>
+        <v>-0.458</v>
       </c>
       <c r="G20" s="1">
-        <v>-0.488</v>
+        <v>-0.596</v>
       </c>
       <c r="H20" s="1">
-        <v>-0.473</v>
+        <v>-0.655</v>
       </c>
       <c r="I20" s="1">
-        <v>-0.391</v>
+        <v>-0.606</v>
       </c>
       <c r="J20" s="1">
-        <v>-0.322</v>
+        <v>-0.49</v>
       </c>
       <c r="K20" s="1">
-        <v>-0.304</v>
+        <v>-0.39</v>
       </c>
       <c r="L20" s="1">
-        <v>-0.334</v>
+        <v>-0.357</v>
       </c>
       <c r="M20" s="1">
-        <v>-0.39</v>
+        <v>-0.385</v>
       </c>
       <c r="N20" s="1">
-        <v>-0.434</v>
+        <v>-0.44</v>
       </c>
       <c r="O20" s="1">
-        <v>-0.44</v>
+        <v>-0.481</v>
       </c>
       <c r="P20" s="1">
-        <v>-0.426</v>
+        <v>-0.501</v>
       </c>
       <c r="Q20" s="1">
-        <v>-0.436</v>
+        <v>-0.531</v>
       </c>
       <c r="R20" s="1">
-        <v>-0.482</v>
+        <v>-0.587</v>
       </c>
       <c r="S20" s="1">
-        <v>-0.532</v>
+        <v>-0.64</v>
       </c>
       <c r="T20" s="1">
-        <v>-0.535</v>
+        <v>-0.652</v>
       </c>
       <c r="U20" s="1">
-        <v>-0.485</v>
+        <v>-0.616</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -1792,64 +1795,64 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>0.027</v>
+        <v>-0.051</v>
       </c>
       <c r="C21" s="1">
-        <v>-0.036</v>
+        <v>-0.113</v>
       </c>
       <c r="D21" s="1">
-        <v>-0.176</v>
+        <v>-0.244</v>
       </c>
       <c r="E21" s="1">
-        <v>-0.326</v>
+        <v>-0.4</v>
       </c>
       <c r="F21" s="1">
-        <v>-0.418</v>
+        <v>-0.549</v>
       </c>
       <c r="G21" s="1">
-        <v>-0.408</v>
+        <v>-0.628</v>
       </c>
       <c r="H21" s="1">
-        <v>-0.336</v>
+        <v>-0.592</v>
       </c>
       <c r="I21" s="1">
-        <v>-0.283</v>
+        <v>-0.479</v>
       </c>
       <c r="J21" s="1">
-        <v>-0.292</v>
+        <v>-0.383</v>
       </c>
       <c r="K21" s="1">
-        <v>-0.362</v>
+        <v>-0.364</v>
       </c>
       <c r="L21" s="1">
-        <v>-0.468</v>
+        <v>-0.415</v>
       </c>
       <c r="M21" s="1">
-        <v>-0.552</v>
+        <v>-0.49</v>
       </c>
       <c r="N21" s="1">
-        <v>-0.573</v>
+        <v>-0.542</v>
       </c>
       <c r="O21" s="1">
-        <v>-0.5590000000000001</v>
+        <v>-0.5649999999999999</v>
       </c>
       <c r="P21" s="1">
-        <v>-0.578</v>
+        <v>-0.602</v>
       </c>
       <c r="Q21" s="1">
-        <v>-0.649</v>
+        <v>-0.673</v>
       </c>
       <c r="R21" s="1">
-        <v>-0.726</v>
+        <v>-0.743</v>
       </c>
       <c r="S21" s="1">
-        <v>-0.735</v>
+        <v>-0.763</v>
       </c>
       <c r="T21" s="1">
-        <v>-0.665</v>
+        <v>-0.72</v>
       </c>
       <c r="U21" s="1">
-        <v>-0.555</v>
+        <v>-0.629</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -1857,64 +1860,64 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>-0.3</v>
+        <v>-0.217</v>
       </c>
       <c r="C22" s="1">
-        <v>-0.376</v>
+        <v>-0.288</v>
       </c>
       <c r="D22" s="1">
-        <v>-0.512</v>
+        <v>-0.438</v>
       </c>
       <c r="E22" s="1">
-        <v>-0.59</v>
+        <v>-0.592</v>
       </c>
       <c r="F22" s="1">
-        <v>-0.5590000000000001</v>
+        <v>-0.6840000000000001</v>
       </c>
       <c r="G22" s="1">
-        <v>-0.467</v>
+        <v>-0.655</v>
       </c>
       <c r="H22" s="1">
-        <v>-0.398</v>
+        <v>-0.534</v>
       </c>
       <c r="I22" s="1">
-        <v>-0.387</v>
+        <v>-0.427</v>
       </c>
       <c r="J22" s="1">
-        <v>-0.43</v>
+        <v>-0.402</v>
       </c>
       <c r="K22" s="1">
-        <v>-0.506</v>
+        <v>-0.454</v>
       </c>
       <c r="L22" s="1">
-        <v>-0.5649999999999999</v>
+        <v>-0.532</v>
       </c>
       <c r="M22" s="1">
-        <v>-0.571</v>
+        <v>-0.586</v>
       </c>
       <c r="N22" s="1">
-        <v>-0.552</v>
+        <v>-0.609</v>
       </c>
       <c r="O22" s="1">
-        <v>-0.5649999999999999</v>
+        <v>-0.647</v>
       </c>
       <c r="P22" s="1">
-        <v>-0.628</v>
+        <v>-0.723</v>
       </c>
       <c r="Q22" s="1">
-        <v>-0.696</v>
+        <v>-0.799</v>
       </c>
       <c r="R22" s="1">
-        <v>-0.702</v>
+        <v>-0.821</v>
       </c>
       <c r="S22" s="1">
-        <v>-0.637</v>
+        <v>-0.774</v>
       </c>
       <c r="T22" s="1">
-        <v>-0.533</v>
+        <v>-0.677</v>
       </c>
       <c r="U22" s="1">
-        <v>-0.416</v>
+        <v>-0.547</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -1922,64 +1925,64 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>-0.484</v>
+        <v>-0.285</v>
       </c>
       <c r="C23" s="1">
-        <v>-0.5620000000000001</v>
+        <v>-0.414</v>
       </c>
       <c r="D23" s="1">
-        <v>-0.612</v>
+        <v>-0.589</v>
       </c>
       <c r="E23" s="1">
-        <v>-0.531</v>
+        <v>-0.651</v>
       </c>
       <c r="F23" s="1">
-        <v>-0.405</v>
+        <v>-0.576</v>
       </c>
       <c r="G23" s="1">
-        <v>-0.329</v>
+        <v>-0.436</v>
       </c>
       <c r="H23" s="1">
-        <v>-0.32</v>
+        <v>-0.343</v>
       </c>
       <c r="I23" s="1">
-        <v>-0.356</v>
+        <v>-0.348</v>
       </c>
       <c r="J23" s="1">
-        <v>-0.413</v>
+        <v>-0.429</v>
       </c>
       <c r="K23" s="1">
-        <v>-0.455</v>
+        <v>-0.525</v>
       </c>
       <c r="L23" s="1">
-        <v>-0.459</v>
+        <v>-0.584</v>
       </c>
       <c r="M23" s="1">
-        <v>-0.444</v>
+        <v>-0.605</v>
       </c>
       <c r="N23" s="1">
-        <v>-0.453</v>
+        <v>-0.64</v>
       </c>
       <c r="O23" s="1">
-        <v>-0.499</v>
+        <v>-0.713</v>
       </c>
       <c r="P23" s="1">
-        <v>-0.544</v>
+        <v>-0.785</v>
       </c>
       <c r="Q23" s="1">
-        <v>-0.541</v>
+        <v>-0.803</v>
       </c>
       <c r="R23" s="1">
-        <v>-0.489</v>
+        <v>-0.75</v>
       </c>
       <c r="S23" s="1">
-        <v>-0.41</v>
+        <v>-0.65</v>
       </c>
       <c r="T23" s="1">
-        <v>-0.318</v>
+        <v>-0.524</v>
       </c>
       <c r="U23" s="1">
-        <v>-0.213</v>
+        <v>-0.374</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -1987,64 +1990,64 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>-0.255</v>
+        <v>-0.095</v>
       </c>
       <c r="C24" s="1">
-        <v>-0.257</v>
+        <v>-0.184</v>
       </c>
       <c r="D24" s="1">
-        <v>-0.214</v>
+        <v>-0.278</v>
       </c>
       <c r="E24" s="1">
-        <v>-0.153</v>
+        <v>-0.267</v>
       </c>
       <c r="F24" s="1">
-        <v>-0.137</v>
+        <v>-0.194</v>
       </c>
       <c r="G24" s="1">
-        <v>-0.181</v>
+        <v>-0.149</v>
       </c>
       <c r="H24" s="1">
-        <v>-0.277</v>
+        <v>-0.189</v>
       </c>
       <c r="I24" s="1">
-        <v>-0.405</v>
+        <v>-0.298</v>
       </c>
       <c r="J24" s="1">
-        <v>-0.512</v>
+        <v>-0.42</v>
       </c>
       <c r="K24" s="1">
-        <v>-0.552</v>
+        <v>-0.5</v>
       </c>
       <c r="L24" s="1">
-        <v>-0.554</v>
+        <v>-0.538</v>
       </c>
       <c r="M24" s="1">
-        <v>-0.587</v>
+        <v>-0.583</v>
       </c>
       <c r="N24" s="1">
-        <v>-0.676</v>
+        <v>-0.664</v>
       </c>
       <c r="O24" s="1">
-        <v>-0.769</v>
+        <v>-0.745</v>
       </c>
       <c r="P24" s="1">
-        <v>-0.786</v>
+        <v>-0.768</v>
       </c>
       <c r="Q24" s="1">
-        <v>-0.714</v>
+        <v>-0.715</v>
       </c>
       <c r="R24" s="1">
-        <v>-0.599</v>
+        <v>-0.614</v>
       </c>
       <c r="S24" s="1">
-        <v>-0.479</v>
+        <v>-0.497</v>
       </c>
       <c r="T24" s="1">
-        <v>-0.359</v>
+        <v>-0.37</v>
       </c>
       <c r="U24" s="1">
-        <v>-0.239</v>
+        <v>-0.243</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -2052,64 +2055,64 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>-0.6850000000000001</v>
+        <v>-0.59</v>
       </c>
       <c r="C25" s="1">
-        <v>-0.606</v>
+        <v>-0.588</v>
       </c>
       <c r="D25" s="1">
-        <v>-0.47</v>
+        <v>-0.516</v>
       </c>
       <c r="E25" s="1">
-        <v>-0.39</v>
+        <v>-0.391</v>
       </c>
       <c r="F25" s="1">
-        <v>-0.376</v>
+        <v>-0.303</v>
       </c>
       <c r="G25" s="1">
-        <v>-0.395</v>
+        <v>-0.285</v>
       </c>
       <c r="H25" s="1">
-        <v>-0.426</v>
+        <v>-0.323</v>
       </c>
       <c r="I25" s="1">
-        <v>-0.447</v>
+        <v>-0.383</v>
       </c>
       <c r="J25" s="1">
-        <v>-0.442</v>
+        <v>-0.43</v>
       </c>
       <c r="K25" s="1">
-        <v>-0.427</v>
+        <v>-0.454</v>
       </c>
       <c r="L25" s="1">
-        <v>-0.436</v>
+        <v>-0.479</v>
       </c>
       <c r="M25" s="1">
-        <v>-0.477</v>
+        <v>-0.516</v>
       </c>
       <c r="N25" s="1">
-        <v>-0.511</v>
+        <v>-0.545</v>
       </c>
       <c r="O25" s="1">
-        <v>-0.502</v>
+        <v>-0.544</v>
       </c>
       <c r="P25" s="1">
-        <v>-0.454</v>
+        <v>-0.51</v>
       </c>
       <c r="Q25" s="1">
-        <v>-0.385</v>
+        <v>-0.446</v>
       </c>
       <c r="R25" s="1">
-        <v>-0.299</v>
+        <v>-0.35</v>
       </c>
       <c r="S25" s="1">
-        <v>-0.196</v>
+        <v>-0.218</v>
       </c>
       <c r="T25" s="1">
-        <v>-0.082</v>
+        <v>-0.076</v>
       </c>
       <c r="U25" s="1">
-        <v>0.015</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -2117,64 +2120,64 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>-0.757</v>
+        <v>-0.726</v>
       </c>
       <c r="C26" s="1">
-        <v>-0.654</v>
+        <v>-0.635</v>
       </c>
       <c r="D26" s="1">
-        <v>-0.534</v>
+        <v>-0.476</v>
       </c>
       <c r="E26" s="1">
-        <v>-0.49</v>
+        <v>-0.376</v>
       </c>
       <c r="F26" s="1">
-        <v>-0.489</v>
+        <v>-0.379</v>
       </c>
       <c r="G26" s="1">
-        <v>-0.507</v>
+        <v>-0.461</v>
       </c>
       <c r="H26" s="1">
-        <v>-0.518</v>
+        <v>-0.5629999999999999</v>
       </c>
       <c r="I26" s="1">
-        <v>-0.5</v>
+        <v>-0.625</v>
       </c>
       <c r="J26" s="1">
-        <v>-0.47</v>
+        <v>-0.643</v>
       </c>
       <c r="K26" s="1">
-        <v>-0.467</v>
+        <v>-0.669</v>
       </c>
       <c r="L26" s="1">
-        <v>-0.499</v>
+        <v>-0.732</v>
       </c>
       <c r="M26" s="1">
-        <v>-0.527</v>
+        <v>-0.793</v>
       </c>
       <c r="N26" s="1">
-        <v>-0.513</v>
+        <v>-0.802</v>
       </c>
       <c r="O26" s="1">
-        <v>-0.464</v>
+        <v>-0.746</v>
       </c>
       <c r="P26" s="1">
-        <v>-0.394</v>
+        <v>-0.647</v>
       </c>
       <c r="Q26" s="1">
-        <v>-0.305</v>
+        <v>-0.52</v>
       </c>
       <c r="R26" s="1">
-        <v>-0.195</v>
+        <v>-0.362</v>
       </c>
       <c r="S26" s="1">
-        <v>-0.07199999999999999</v>
+        <v>-0.188</v>
       </c>
       <c r="T26" s="1">
-        <v>0.033</v>
+        <v>-0.046</v>
       </c>
       <c r="U26" s="1">
-        <v>0.096</v>
+        <v>0.041</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -2182,64 +2185,64 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>-0.407</v>
+        <v>-0.344</v>
       </c>
       <c r="C27" s="1">
-        <v>-0.349</v>
+        <v>-0.241</v>
       </c>
       <c r="D27" s="1">
-        <v>-0.321</v>
+        <v>-0.141</v>
       </c>
       <c r="E27" s="1">
-        <v>-0.373</v>
+        <v>-0.17</v>
       </c>
       <c r="F27" s="1">
-        <v>-0.453</v>
+        <v>-0.287</v>
       </c>
       <c r="G27" s="1">
-        <v>-0.499</v>
+        <v>-0.413</v>
       </c>
       <c r="H27" s="1">
-        <v>-0.479</v>
+        <v>-0.483</v>
       </c>
       <c r="I27" s="1">
-        <v>-0.436</v>
+        <v>-0.507</v>
       </c>
       <c r="J27" s="1">
-        <v>-0.425</v>
+        <v>-0.534</v>
       </c>
       <c r="K27" s="1">
-        <v>-0.449</v>
+        <v>-0.588</v>
       </c>
       <c r="L27" s="1">
-        <v>-0.468</v>
+        <v>-0.641</v>
       </c>
       <c r="M27" s="1">
-        <v>-0.448</v>
+        <v>-0.653</v>
       </c>
       <c r="N27" s="1">
-        <v>-0.393</v>
+        <v>-0.606</v>
       </c>
       <c r="O27" s="1">
-        <v>-0.327</v>
+        <v>-0.517</v>
       </c>
       <c r="P27" s="1">
-        <v>-0.254</v>
+        <v>-0.405</v>
       </c>
       <c r="Q27" s="1">
-        <v>-0.168</v>
+        <v>-0.277</v>
       </c>
       <c r="R27" s="1">
-        <v>-0.074</v>
+        <v>-0.149</v>
       </c>
       <c r="S27" s="1">
-        <v>0.007</v>
+        <v>-0.054</v>
       </c>
       <c r="T27" s="1">
-        <v>0.058</v>
+        <v>-0.001</v>
       </c>
       <c r="U27" s="1">
-        <v>0.09</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -2247,64 +2250,64 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>0.074</v>
+        <v>0.128</v>
       </c>
       <c r="C28" s="1">
-        <v>0.029</v>
+        <v>0.128</v>
       </c>
       <c r="D28" s="1">
-        <v>-0.075</v>
+        <v>0.079</v>
       </c>
       <c r="E28" s="1">
-        <v>-0.198</v>
+        <v>-0.03</v>
       </c>
       <c r="F28" s="1">
-        <v>-0.287</v>
+        <v>-0.146</v>
       </c>
       <c r="G28" s="1">
-        <v>-0.309</v>
+        <v>-0.225</v>
       </c>
       <c r="H28" s="1">
-        <v>-0.301</v>
+        <v>-0.266</v>
       </c>
       <c r="I28" s="1">
-        <v>-0.311</v>
+        <v>-0.299</v>
       </c>
       <c r="J28" s="1">
-        <v>-0.345</v>
+        <v>-0.341</v>
       </c>
       <c r="K28" s="1">
-        <v>-0.373</v>
+        <v>-0.381</v>
       </c>
       <c r="L28" s="1">
-        <v>-0.363</v>
+        <v>-0.396</v>
       </c>
       <c r="M28" s="1">
-        <v>-0.32</v>
+        <v>-0.372</v>
       </c>
       <c r="N28" s="1">
-        <v>-0.267</v>
+        <v>-0.315</v>
       </c>
       <c r="O28" s="1">
-        <v>-0.216</v>
+        <v>-0.244</v>
       </c>
       <c r="P28" s="1">
-        <v>-0.166</v>
+        <v>-0.174</v>
       </c>
       <c r="Q28" s="1">
-        <v>-0.116</v>
+        <v>-0.114</v>
       </c>
       <c r="R28" s="1">
-        <v>-0.073</v>
+        <v>-0.076</v>
       </c>
       <c r="S28" s="1">
-        <v>-0.043</v>
+        <v>-0.06</v>
       </c>
       <c r="T28" s="1">
-        <v>-0.024</v>
+        <v>-0.052</v>
       </c>
       <c r="U28" s="1">
-        <v>-0.008</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -2312,64 +2315,129 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>-0.127</v>
+        <v>-0.118</v>
       </c>
       <c r="C29" s="1">
-        <v>-0.169</v>
+        <v>-0.106</v>
       </c>
       <c r="D29" s="1">
-        <v>-0.239</v>
+        <v>-0.117</v>
       </c>
       <c r="E29" s="1">
-        <v>-0.268</v>
+        <v>-0.145</v>
       </c>
       <c r="F29" s="1">
-        <v>-0.239</v>
+        <v>-0.157</v>
       </c>
       <c r="G29" s="1">
-        <v>-0.199</v>
+        <v>-0.158</v>
       </c>
       <c r="H29" s="1">
-        <v>-0.182</v>
+        <v>-0.158</v>
       </c>
       <c r="I29" s="1">
-        <v>-0.178</v>
+        <v>-0.154</v>
       </c>
       <c r="J29" s="1">
-        <v>-0.165</v>
+        <v>-0.146</v>
       </c>
       <c r="K29" s="1">
-        <v>-0.136</v>
+        <v>-0.139</v>
       </c>
       <c r="L29" s="1">
-        <v>-0.105</v>
+        <v>-0.13</v>
       </c>
       <c r="M29" s="1">
-        <v>-0.082</v>
+        <v>-0.108</v>
       </c>
       <c r="N29" s="1">
-        <v>-0.064</v>
+        <v>-0.067</v>
       </c>
       <c r="O29" s="1">
-        <v>-0.041</v>
+        <v>-0.015</v>
       </c>
       <c r="P29" s="1">
-        <v>-0.014</v>
+        <v>0.03</v>
       </c>
       <c r="Q29" s="1">
-        <v>0.011</v>
+        <v>0.054</v>
       </c>
       <c r="R29" s="1">
-        <v>0.027</v>
+        <v>0.057</v>
       </c>
       <c r="S29" s="1">
-        <v>0.036</v>
+        <v>0.055</v>
       </c>
       <c r="T29" s="1">
-        <v>0.048</v>
+        <v>0.065</v>
       </c>
       <c r="U29" s="1">
-        <v>0.065</v>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>-0.045</v>
+      </c>
+      <c r="C30" s="1">
+        <v>-0.062</v>
+      </c>
+      <c r="D30" s="1">
+        <v>-0.093</v>
+      </c>
+      <c r="E30" s="1">
+        <v>-0.112</v>
+      </c>
+      <c r="F30" s="1">
+        <v>-0.126</v>
+      </c>
+      <c r="G30" s="1">
+        <v>-0.151</v>
+      </c>
+      <c r="H30" s="1">
+        <v>-0.186</v>
+      </c>
+      <c r="I30" s="1">
+        <v>-0.217</v>
+      </c>
+      <c r="J30" s="1">
+        <v>-0.232</v>
+      </c>
+      <c r="K30" s="1">
+        <v>-0.221</v>
+      </c>
+      <c r="L30" s="1">
+        <v>-0.185</v>
+      </c>
+      <c r="M30" s="1">
+        <v>-0.143</v>
+      </c>
+      <c r="N30" s="1">
+        <v>-0.111</v>
+      </c>
+      <c r="O30" s="1">
+        <v>-0.095</v>
+      </c>
+      <c r="P30" s="1">
+        <v>-0.093</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>-0.098</v>
+      </c>
+      <c r="R30" s="1">
+        <v>-0.104</v>
+      </c>
+      <c r="S30" s="1">
+        <v>-0.109</v>
+      </c>
+      <c r="T30" s="1">
+        <v>-0.117</v>
+      </c>
+      <c r="U30" s="1">
+        <v>-0.122</v>
       </c>
     </row>
   </sheetData>
@@ -2387,22 +2455,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
XRO forecast sep 2025
</commit_message>
<xml_diff>
--- a/content/climate/XRO/XRO_ENSO_fcst.xlsx
+++ b/content/climate/XRO/XRO_ENSO_fcst.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>init</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>2025-07</t>
+  </si>
+  <si>
+    <t>2025-08</t>
   </si>
   <si>
     <t>Readme</t>
@@ -487,7 +490,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,7 +501,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2">
         <v>0</v>
@@ -584,37 +587,37 @@
         <v>0.258</v>
       </c>
       <c r="H2" s="1">
-        <v>0.5669999999999999</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="I2" s="1">
-        <v>0.762</v>
+        <v>0.763</v>
       </c>
       <c r="J2" s="1">
-        <v>0.9399999999999999</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="K2" s="1">
-        <v>1.211</v>
+        <v>1.213</v>
       </c>
       <c r="L2" s="1">
-        <v>1.563</v>
+        <v>1.564</v>
       </c>
       <c r="M2" s="1">
-        <v>1.828</v>
+        <v>1.829</v>
       </c>
       <c r="N2" s="1">
-        <v>1.884</v>
+        <v>1.885</v>
       </c>
       <c r="O2" s="1">
-        <v>1.754</v>
+        <v>1.755</v>
       </c>
       <c r="P2" s="1">
-        <v>1.506</v>
+        <v>1.507</v>
       </c>
       <c r="Q2" s="1">
-        <v>1.201</v>
+        <v>1.202</v>
       </c>
       <c r="R2" s="1">
-        <v>0.884</v>
+        <v>0.885</v>
       </c>
       <c r="S2" s="1">
         <v>0.593</v>
@@ -643,46 +646,46 @@
         <v>-0.023</v>
       </c>
       <c r="F3" s="1">
-        <v>0.291</v>
+        <v>0.292</v>
       </c>
       <c r="G3" s="1">
-        <v>0.521</v>
+        <v>0.522</v>
       </c>
       <c r="H3" s="1">
-        <v>0.66</v>
+        <v>0.661</v>
       </c>
       <c r="I3" s="1">
-        <v>0.779</v>
+        <v>0.781</v>
       </c>
       <c r="J3" s="1">
-        <v>0.953</v>
+        <v>0.954</v>
       </c>
       <c r="K3" s="1">
-        <v>1.169</v>
+        <v>1.171</v>
       </c>
       <c r="L3" s="1">
-        <v>1.324</v>
+        <v>1.326</v>
       </c>
       <c r="M3" s="1">
-        <v>1.334</v>
+        <v>1.336</v>
       </c>
       <c r="N3" s="1">
-        <v>1.214</v>
+        <v>1.215</v>
       </c>
       <c r="O3" s="1">
-        <v>1.026</v>
+        <v>1.027</v>
       </c>
       <c r="P3" s="1">
-        <v>0.8159999999999999</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="Q3" s="1">
-        <v>0.592</v>
+        <v>0.593</v>
       </c>
       <c r="R3" s="1">
-        <v>0.372</v>
+        <v>0.373</v>
       </c>
       <c r="S3" s="1">
-        <v>0.184</v>
+        <v>0.185</v>
       </c>
       <c r="T3" s="1">
         <v>0.047</v>
@@ -705,46 +708,46 @@
         <v>0.275</v>
       </c>
       <c r="E4" s="1">
-        <v>0.481</v>
+        <v>0.482</v>
       </c>
       <c r="F4" s="1">
-        <v>0.606</v>
+        <v>0.607</v>
       </c>
       <c r="G4" s="1">
-        <v>0.661</v>
+        <v>0.662</v>
       </c>
       <c r="H4" s="1">
-        <v>0.716</v>
+        <v>0.717</v>
       </c>
       <c r="I4" s="1">
-        <v>0.824</v>
+        <v>0.826</v>
       </c>
       <c r="J4" s="1">
-        <v>0.971</v>
+        <v>0.972</v>
       </c>
       <c r="K4" s="1">
-        <v>1.071</v>
+        <v>1.073</v>
       </c>
       <c r="L4" s="1">
-        <v>1.055</v>
+        <v>1.057</v>
       </c>
       <c r="M4" s="1">
-        <v>0.9360000000000001</v>
+        <v>0.9379999999999999</v>
       </c>
       <c r="N4" s="1">
-        <v>0.781</v>
+        <v>0.783</v>
       </c>
       <c r="O4" s="1">
-        <v>0.622</v>
+        <v>0.623</v>
       </c>
       <c r="P4" s="1">
-        <v>0.445</v>
+        <v>0.446</v>
       </c>
       <c r="Q4" s="1">
         <v>0.253</v>
       </c>
       <c r="R4" s="1">
-        <v>0.077</v>
+        <v>0.078</v>
       </c>
       <c r="S4" s="1">
         <v>-0.055</v>
@@ -764,7 +767,7 @@
         <v>0.182</v>
       </c>
       <c r="C5" s="1">
-        <v>0.333</v>
+        <v>0.334</v>
       </c>
       <c r="D5" s="1">
         <v>0.571</v>
@@ -776,28 +779,28 @@
         <v>0.842</v>
       </c>
       <c r="G5" s="1">
-        <v>0.925</v>
+        <v>0.926</v>
       </c>
       <c r="H5" s="1">
-        <v>1.045</v>
+        <v>1.046</v>
       </c>
       <c r="I5" s="1">
-        <v>1.191</v>
+        <v>1.192</v>
       </c>
       <c r="J5" s="1">
-        <v>1.272</v>
+        <v>1.273</v>
       </c>
       <c r="K5" s="1">
-        <v>1.217</v>
+        <v>1.218</v>
       </c>
       <c r="L5" s="1">
-        <v>1.057</v>
+        <v>1.058</v>
       </c>
       <c r="M5" s="1">
-        <v>0.875</v>
+        <v>0.876</v>
       </c>
       <c r="N5" s="1">
-        <v>0.697</v>
+        <v>0.698</v>
       </c>
       <c r="O5" s="1">
         <v>0.489</v>
@@ -809,7 +812,7 @@
         <v>0.022</v>
       </c>
       <c r="R5" s="1">
-        <v>-0.154</v>
+        <v>-0.153</v>
       </c>
       <c r="S5" s="1">
         <v>-0.27</v>
@@ -818,7 +821,7 @@
         <v>-0.362</v>
       </c>
       <c r="U5" s="1">
-        <v>-0.461</v>
+        <v>-0.46</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -841,22 +844,22 @@
         <v>1.056</v>
       </c>
       <c r="G6" s="1">
-        <v>1.182</v>
+        <v>1.183</v>
       </c>
       <c r="H6" s="1">
         <v>1.328</v>
       </c>
       <c r="I6" s="1">
-        <v>1.392</v>
+        <v>1.393</v>
       </c>
       <c r="J6" s="1">
         <v>1.308</v>
       </c>
       <c r="K6" s="1">
-        <v>1.117</v>
+        <v>1.118</v>
       </c>
       <c r="L6" s="1">
-        <v>0.915</v>
+        <v>0.916</v>
       </c>
       <c r="M6" s="1">
         <v>0.725</v>
@@ -868,7 +871,7 @@
         <v>0.241</v>
       </c>
       <c r="P6" s="1">
-        <v>-0.008999999999999999</v>
+        <v>-0.008</v>
       </c>
       <c r="Q6" s="1">
         <v>-0.201</v>
@@ -883,7 +886,7 @@
         <v>-0.537</v>
       </c>
       <c r="U6" s="1">
-        <v>-0.64</v>
+        <v>-0.639</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -894,7 +897,7 @@
         <v>0.904</v>
       </c>
       <c r="C7" s="1">
-        <v>1.006</v>
+        <v>1.007</v>
       </c>
       <c r="D7" s="1">
         <v>1.129</v>
@@ -906,16 +909,16 @@
         <v>1.344</v>
       </c>
       <c r="G7" s="1">
-        <v>1.46</v>
+        <v>1.461</v>
       </c>
       <c r="H7" s="1">
-        <v>1.48</v>
+        <v>1.481</v>
       </c>
       <c r="I7" s="1">
-        <v>1.355</v>
+        <v>1.357</v>
       </c>
       <c r="J7" s="1">
-        <v>1.14</v>
+        <v>1.141</v>
       </c>
       <c r="K7" s="1">
         <v>0.926</v>
@@ -930,7 +933,7 @@
         <v>0.151</v>
       </c>
       <c r="O7" s="1">
-        <v>-0.14</v>
+        <v>-0.139</v>
       </c>
       <c r="P7" s="1">
         <v>-0.352</v>
@@ -962,31 +965,31 @@
         <v>1.163</v>
       </c>
       <c r="D8" s="1">
-        <v>1.33</v>
+        <v>1.331</v>
       </c>
       <c r="E8" s="1">
-        <v>1.481</v>
+        <v>1.482</v>
       </c>
       <c r="F8" s="1">
-        <v>1.573</v>
+        <v>1.574</v>
       </c>
       <c r="G8" s="1">
-        <v>1.532</v>
+        <v>1.534</v>
       </c>
       <c r="H8" s="1">
-        <v>1.345</v>
+        <v>1.347</v>
       </c>
       <c r="I8" s="1">
-        <v>1.092</v>
+        <v>1.093</v>
       </c>
       <c r="J8" s="1">
-        <v>0.867</v>
+        <v>0.868</v>
       </c>
       <c r="K8" s="1">
-        <v>0.658</v>
+        <v>0.659</v>
       </c>
       <c r="L8" s="1">
-        <v>0.386</v>
+        <v>0.387</v>
       </c>
       <c r="M8" s="1">
         <v>0.055</v>
@@ -995,7 +998,7 @@
         <v>-0.259</v>
       </c>
       <c r="O8" s="1">
-        <v>-0.48</v>
+        <v>-0.479</v>
       </c>
       <c r="P8" s="1">
         <v>-0.599</v>
@@ -1027,25 +1030,25 @@
         <v>1.447</v>
       </c>
       <c r="D9" s="1">
-        <v>1.659</v>
+        <v>1.66</v>
       </c>
       <c r="E9" s="1">
-        <v>1.758</v>
+        <v>1.759</v>
       </c>
       <c r="F9" s="1">
-        <v>1.682</v>
+        <v>1.683</v>
       </c>
       <c r="G9" s="1">
-        <v>1.461</v>
+        <v>1.462</v>
       </c>
       <c r="H9" s="1">
-        <v>1.191</v>
+        <v>1.192</v>
       </c>
       <c r="I9" s="1">
-        <v>0.953</v>
+        <v>0.955</v>
       </c>
       <c r="J9" s="1">
-        <v>0.714</v>
+        <v>0.715</v>
       </c>
       <c r="K9" s="1">
         <v>0.393</v>
@@ -1054,10 +1057,10 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="M9" s="1">
-        <v>-0.347</v>
+        <v>-0.346</v>
       </c>
       <c r="N9" s="1">
-        <v>-0.585</v>
+        <v>-0.584</v>
       </c>
       <c r="O9" s="1">
         <v>-0.703</v>
@@ -1092,22 +1095,22 @@
         <v>1.696</v>
       </c>
       <c r="D10" s="1">
-        <v>1.856</v>
+        <v>1.857</v>
       </c>
       <c r="E10" s="1">
-        <v>1.821</v>
+        <v>1.822</v>
       </c>
       <c r="F10" s="1">
-        <v>1.609</v>
+        <v>1.61</v>
       </c>
       <c r="G10" s="1">
-        <v>1.331</v>
+        <v>1.332</v>
       </c>
       <c r="H10" s="1">
-        <v>1.074</v>
+        <v>1.075</v>
       </c>
       <c r="I10" s="1">
-        <v>0.8139999999999999</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="J10" s="1">
         <v>0.481</v>
@@ -1116,10 +1119,10 @@
         <v>0.093</v>
       </c>
       <c r="L10" s="1">
-        <v>-0.264</v>
+        <v>-0.263</v>
       </c>
       <c r="M10" s="1">
-        <v>-0.508</v>
+        <v>-0.507</v>
       </c>
       <c r="N10" s="1">
         <v>-0.636</v>
@@ -1157,28 +1160,28 @@
         <v>1.722</v>
       </c>
       <c r="D11" s="1">
-        <v>1.796</v>
+        <v>1.797</v>
       </c>
       <c r="E11" s="1">
         <v>1.647</v>
       </c>
       <c r="F11" s="1">
-        <v>1.391</v>
+        <v>1.392</v>
       </c>
       <c r="G11" s="1">
         <v>1.132</v>
       </c>
       <c r="H11" s="1">
-        <v>0.864</v>
+        <v>0.865</v>
       </c>
       <c r="I11" s="1">
-        <v>0.538</v>
+        <v>0.539</v>
       </c>
       <c r="J11" s="1">
-        <v>0.174</v>
+        <v>0.175</v>
       </c>
       <c r="K11" s="1">
-        <v>-0.156</v>
+        <v>-0.155</v>
       </c>
       <c r="L11" s="1">
         <v>-0.385</v>
@@ -1199,16 +1202,16 @@
         <v>-0.9409999999999999</v>
       </c>
       <c r="R11" s="1">
-        <v>-0.868</v>
+        <v>-0.867</v>
       </c>
       <c r="S11" s="1">
-        <v>-0.719</v>
+        <v>-0.718</v>
       </c>
       <c r="T11" s="1">
         <v>-0.582</v>
       </c>
       <c r="U11" s="1">
-        <v>-0.491</v>
+        <v>-0.49</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1225,10 +1228,10 @@
         <v>1.666</v>
       </c>
       <c r="E12" s="1">
-        <v>1.417</v>
+        <v>1.418</v>
       </c>
       <c r="F12" s="1">
-        <v>1.158</v>
+        <v>1.159</v>
       </c>
       <c r="G12" s="1">
         <v>0.863</v>
@@ -1240,10 +1243,10 @@
         <v>0.075</v>
       </c>
       <c r="J12" s="1">
-        <v>-0.293</v>
+        <v>-0.292</v>
       </c>
       <c r="K12" s="1">
-        <v>-0.538</v>
+        <v>-0.537</v>
       </c>
       <c r="L12" s="1">
         <v>-0.666</v>
@@ -1255,13 +1258,13 @@
         <v>-0.929</v>
       </c>
       <c r="O12" s="1">
-        <v>-1.091</v>
+        <v>-1.09</v>
       </c>
       <c r="P12" s="1">
         <v>-1.155</v>
       </c>
       <c r="Q12" s="1">
-        <v>-1.062</v>
+        <v>-1.061</v>
       </c>
       <c r="R12" s="1">
         <v>-0.88</v>
@@ -1296,22 +1299,22 @@
         <v>0.956</v>
       </c>
       <c r="G13" s="1">
-        <v>0.533</v>
+        <v>0.534</v>
       </c>
       <c r="H13" s="1">
         <v>0.067</v>
       </c>
       <c r="I13" s="1">
-        <v>-0.354</v>
+        <v>-0.353</v>
       </c>
       <c r="J13" s="1">
         <v>-0.642</v>
       </c>
       <c r="K13" s="1">
-        <v>-0.795</v>
+        <v>-0.794</v>
       </c>
       <c r="L13" s="1">
-        <v>-0.918</v>
+        <v>-0.917</v>
       </c>
       <c r="M13" s="1">
         <v>-1.089</v>
@@ -1349,10 +1352,10 @@
         <v>1.78</v>
       </c>
       <c r="C14" s="1">
-        <v>1.667</v>
+        <v>1.668</v>
       </c>
       <c r="D14" s="1">
-        <v>1.388</v>
+        <v>1.389</v>
       </c>
       <c r="E14" s="1">
         <v>0.989</v>
@@ -1382,28 +1385,28 @@
         <v>-1.467</v>
       </c>
       <c r="N14" s="1">
-        <v>-1.545</v>
+        <v>-1.546</v>
       </c>
       <c r="O14" s="1">
-        <v>-1.407</v>
+        <v>-1.408</v>
       </c>
       <c r="P14" s="1">
         <v>-1.159</v>
       </c>
       <c r="Q14" s="1">
-        <v>-0.947</v>
+        <v>-0.948</v>
       </c>
       <c r="R14" s="1">
-        <v>-0.8129999999999999</v>
+        <v>-0.8139999999999999</v>
       </c>
       <c r="S14" s="1">
         <v>-0.731</v>
       </c>
       <c r="T14" s="1">
-        <v>-0.673</v>
+        <v>-0.672</v>
       </c>
       <c r="U14" s="1">
-        <v>-0.622</v>
+        <v>-0.621</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1441,22 +1444,22 @@
         <v>-1.319</v>
       </c>
       <c r="L15" s="1">
-        <v>-1.539</v>
+        <v>-1.54</v>
       </c>
       <c r="M15" s="1">
         <v>-1.632</v>
       </c>
       <c r="N15" s="1">
-        <v>-1.498</v>
+        <v>-1.499</v>
       </c>
       <c r="O15" s="1">
-        <v>-1.24</v>
+        <v>-1.241</v>
       </c>
       <c r="P15" s="1">
-        <v>-1.013</v>
+        <v>-1.014</v>
       </c>
       <c r="Q15" s="1">
-        <v>-0.87</v>
+        <v>-0.871</v>
       </c>
       <c r="R15" s="1">
         <v>-0.789</v>
@@ -1468,7 +1471,7 @@
         <v>-0.694</v>
       </c>
       <c r="U15" s="1">
-        <v>-0.657</v>
+        <v>-0.656</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1503,10 +1506,10 @@
         <v>-1.171</v>
       </c>
       <c r="K16" s="1">
-        <v>-1.367</v>
+        <v>-1.368</v>
       </c>
       <c r="L16" s="1">
-        <v>-1.459</v>
+        <v>-1.46</v>
       </c>
       <c r="M16" s="1">
         <v>-1.353</v>
@@ -1515,7 +1518,7 @@
         <v>-1.126</v>
       </c>
       <c r="O16" s="1">
-        <v>-0.914</v>
+        <v>-0.915</v>
       </c>
       <c r="P16" s="1">
         <v>-0.773</v>
@@ -1530,10 +1533,10 @@
         <v>-0.605</v>
       </c>
       <c r="T16" s="1">
-        <v>-0.577</v>
+        <v>-0.576</v>
       </c>
       <c r="U16" s="1">
-        <v>-0.575</v>
+        <v>-0.574</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -1571,7 +1574,7 @@
         <v>-1.411</v>
       </c>
       <c r="L17" s="1">
-        <v>-1.312</v>
+        <v>-1.313</v>
       </c>
       <c r="M17" s="1">
         <v>-1.093</v>
@@ -1583,22 +1586,22 @@
         <v>-0.74</v>
       </c>
       <c r="P17" s="1">
-        <v>-0.653</v>
+        <v>-0.654</v>
       </c>
       <c r="Q17" s="1">
         <v>-0.607</v>
       </c>
       <c r="R17" s="1">
-        <v>-0.579</v>
+        <v>-0.578</v>
       </c>
       <c r="S17" s="1">
         <v>-0.5570000000000001</v>
       </c>
       <c r="T17" s="1">
-        <v>-0.5580000000000001</v>
+        <v>-0.5570000000000001</v>
       </c>
       <c r="U17" s="1">
-        <v>-0.586</v>
+        <v>-0.585</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -1621,7 +1624,7 @@
         <v>-0.9370000000000001</v>
       </c>
       <c r="G18" s="1">
-        <v>-1.043</v>
+        <v>-1.042</v>
       </c>
       <c r="H18" s="1">
         <v>-1.204</v>
@@ -1630,19 +1633,19 @@
         <v>-1.384</v>
       </c>
       <c r="J18" s="1">
-        <v>-1.462</v>
+        <v>-1.463</v>
       </c>
       <c r="K18" s="1">
-        <v>-1.357</v>
+        <v>-1.358</v>
       </c>
       <c r="L18" s="1">
-        <v>-1.138</v>
+        <v>-1.139</v>
       </c>
       <c r="M18" s="1">
-        <v>-0.924</v>
+        <v>-0.925</v>
       </c>
       <c r="N18" s="1">
-        <v>-0.76</v>
+        <v>-0.761</v>
       </c>
       <c r="O18" s="1">
         <v>-0.642</v>
@@ -1660,10 +1663,10 @@
         <v>-0.48</v>
       </c>
       <c r="T18" s="1">
-        <v>-0.49</v>
+        <v>-0.489</v>
       </c>
       <c r="U18" s="1">
-        <v>-0.493</v>
+        <v>-0.492</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -1680,10 +1683,10 @@
         <v>-0.302</v>
       </c>
       <c r="E19" s="1">
-        <v>-0.498</v>
+        <v>-0.497</v>
       </c>
       <c r="F19" s="1">
-        <v>-0.65</v>
+        <v>-0.649</v>
       </c>
       <c r="G19" s="1">
         <v>-0.823</v>
@@ -1713,7 +1716,7 @@
         <v>-0.5610000000000001</v>
       </c>
       <c r="P19" s="1">
-        <v>-0.57</v>
+        <v>-0.569</v>
       </c>
       <c r="Q19" s="1">
         <v>-0.5659999999999999</v>
@@ -1722,13 +1725,13 @@
         <v>-0.581</v>
       </c>
       <c r="S19" s="1">
-        <v>-0.63</v>
+        <v>-0.629</v>
       </c>
       <c r="T19" s="1">
         <v>-0.676</v>
       </c>
       <c r="U19" s="1">
-        <v>-0.6830000000000001</v>
+        <v>-0.6820000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -1754,7 +1757,7 @@
         <v>-0.588</v>
       </c>
       <c r="H20" s="1">
-        <v>-0.647</v>
+        <v>-0.646</v>
       </c>
       <c r="I20" s="1">
         <v>-0.598</v>
@@ -1763,37 +1766,37 @@
         <v>-0.482</v>
       </c>
       <c r="K20" s="1">
-        <v>-0.383</v>
+        <v>-0.382</v>
       </c>
       <c r="L20" s="1">
         <v>-0.351</v>
       </c>
       <c r="M20" s="1">
-        <v>-0.383</v>
+        <v>-0.382</v>
       </c>
       <c r="N20" s="1">
         <v>-0.44</v>
       </c>
       <c r="O20" s="1">
-        <v>-0.484</v>
+        <v>-0.483</v>
       </c>
       <c r="P20" s="1">
-        <v>-0.505</v>
+        <v>-0.504</v>
       </c>
       <c r="Q20" s="1">
         <v>-0.535</v>
       </c>
       <c r="R20" s="1">
-        <v>-0.593</v>
+        <v>-0.592</v>
       </c>
       <c r="S20" s="1">
-        <v>-0.647</v>
+        <v>-0.646</v>
       </c>
       <c r="T20" s="1">
-        <v>-0.66</v>
+        <v>-0.659</v>
       </c>
       <c r="U20" s="1">
-        <v>-0.623</v>
+        <v>-0.622</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -1813,7 +1816,7 @@
         <v>-0.395</v>
       </c>
       <c r="F21" s="1">
-        <v>-0.542</v>
+        <v>-0.541</v>
       </c>
       <c r="G21" s="1">
         <v>-0.619</v>
@@ -1831,13 +1834,13 @@
         <v>-0.359</v>
       </c>
       <c r="L21" s="1">
-        <v>-0.413</v>
+        <v>-0.412</v>
       </c>
       <c r="M21" s="1">
-        <v>-0.49</v>
+        <v>-0.489</v>
       </c>
       <c r="N21" s="1">
-        <v>-0.544</v>
+        <v>-0.543</v>
       </c>
       <c r="O21" s="1">
         <v>-0.5679999999999999</v>
@@ -1846,16 +1849,16 @@
         <v>-0.605</v>
       </c>
       <c r="Q21" s="1">
-        <v>-0.678</v>
+        <v>-0.677</v>
       </c>
       <c r="R21" s="1">
-        <v>-0.749</v>
+        <v>-0.748</v>
       </c>
       <c r="S21" s="1">
-        <v>-0.77</v>
+        <v>-0.769</v>
       </c>
       <c r="T21" s="1">
-        <v>-0.725</v>
+        <v>-0.724</v>
       </c>
       <c r="U21" s="1">
         <v>-0.632</v>
@@ -1896,7 +1899,7 @@
         <v>-0.451</v>
       </c>
       <c r="L22" s="1">
-        <v>-0.532</v>
+        <v>-0.531</v>
       </c>
       <c r="M22" s="1">
         <v>-0.587</v>
@@ -1905,25 +1908,25 @@
         <v>-0.611</v>
       </c>
       <c r="O22" s="1">
-        <v>-0.65</v>
+        <v>-0.649</v>
       </c>
       <c r="P22" s="1">
-        <v>-0.727</v>
+        <v>-0.726</v>
       </c>
       <c r="Q22" s="1">
-        <v>-0.804</v>
+        <v>-0.803</v>
       </c>
       <c r="R22" s="1">
-        <v>-0.827</v>
+        <v>-0.826</v>
       </c>
       <c r="S22" s="1">
-        <v>-0.779</v>
+        <v>-0.778</v>
       </c>
       <c r="T22" s="1">
         <v>-0.679</v>
       </c>
       <c r="U22" s="1">
-        <v>-0.55</v>
+        <v>-0.549</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -1940,7 +1943,7 @@
         <v>-0.586</v>
       </c>
       <c r="E23" s="1">
-        <v>-0.647</v>
+        <v>-0.646</v>
       </c>
       <c r="F23" s="1">
         <v>-0.571</v>
@@ -1952,43 +1955,43 @@
         <v>-0.337</v>
       </c>
       <c r="I23" s="1">
-        <v>-0.344</v>
+        <v>-0.343</v>
       </c>
       <c r="J23" s="1">
         <v>-0.426</v>
       </c>
       <c r="K23" s="1">
-        <v>-0.525</v>
+        <v>-0.524</v>
       </c>
       <c r="L23" s="1">
-        <v>-0.585</v>
+        <v>-0.584</v>
       </c>
       <c r="M23" s="1">
-        <v>-0.607</v>
+        <v>-0.606</v>
       </c>
       <c r="N23" s="1">
-        <v>-0.642</v>
+        <v>-0.641</v>
       </c>
       <c r="O23" s="1">
         <v>-0.715</v>
       </c>
       <c r="P23" s="1">
-        <v>-0.789</v>
+        <v>-0.788</v>
       </c>
       <c r="Q23" s="1">
-        <v>-0.8070000000000001</v>
+        <v>-0.806</v>
       </c>
       <c r="R23" s="1">
-        <v>-0.753</v>
+        <v>-0.752</v>
       </c>
       <c r="S23" s="1">
-        <v>-0.652</v>
+        <v>-0.651</v>
       </c>
       <c r="T23" s="1">
-        <v>-0.526</v>
+        <v>-0.525</v>
       </c>
       <c r="U23" s="1">
-        <v>-0.377</v>
+        <v>-0.376</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -1999,7 +2002,7 @@
         <v>-0.095</v>
       </c>
       <c r="C24" s="1">
-        <v>-0.184</v>
+        <v>-0.183</v>
       </c>
       <c r="D24" s="1">
         <v>-0.277</v>
@@ -2008,7 +2011,7 @@
         <v>-0.266</v>
       </c>
       <c r="F24" s="1">
-        <v>-0.193</v>
+        <v>-0.192</v>
       </c>
       <c r="G24" s="1">
         <v>-0.147</v>
@@ -2017,43 +2020,43 @@
         <v>-0.187</v>
       </c>
       <c r="I24" s="1">
-        <v>-0.298</v>
+        <v>-0.297</v>
       </c>
       <c r="J24" s="1">
-        <v>-0.421</v>
+        <v>-0.42</v>
       </c>
       <c r="K24" s="1">
-        <v>-0.502</v>
+        <v>-0.501</v>
       </c>
       <c r="L24" s="1">
         <v>-0.539</v>
       </c>
       <c r="M24" s="1">
-        <v>-0.585</v>
+        <v>-0.584</v>
       </c>
       <c r="N24" s="1">
-        <v>-0.667</v>
+        <v>-0.665</v>
       </c>
       <c r="O24" s="1">
-        <v>-0.748</v>
+        <v>-0.747</v>
       </c>
       <c r="P24" s="1">
-        <v>-0.772</v>
+        <v>-0.77</v>
       </c>
       <c r="Q24" s="1">
-        <v>-0.718</v>
+        <v>-0.717</v>
       </c>
       <c r="R24" s="1">
         <v>-0.615</v>
       </c>
       <c r="S24" s="1">
-        <v>-0.498</v>
+        <v>-0.497</v>
       </c>
       <c r="T24" s="1">
-        <v>-0.373</v>
+        <v>-0.372</v>
       </c>
       <c r="U24" s="1">
-        <v>-0.248</v>
+        <v>-0.247</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -2076,49 +2079,49 @@
         <v>-0.301</v>
       </c>
       <c r="G25" s="1">
-        <v>-0.283</v>
+        <v>-0.282</v>
       </c>
       <c r="H25" s="1">
         <v>-0.321</v>
       </c>
       <c r="I25" s="1">
-        <v>-0.383</v>
+        <v>-0.382</v>
       </c>
       <c r="J25" s="1">
-        <v>-0.431</v>
+        <v>-0.43</v>
       </c>
       <c r="K25" s="1">
-        <v>-0.455</v>
+        <v>-0.454</v>
       </c>
       <c r="L25" s="1">
-        <v>-0.48</v>
+        <v>-0.479</v>
       </c>
       <c r="M25" s="1">
-        <v>-0.518</v>
+        <v>-0.516</v>
       </c>
       <c r="N25" s="1">
-        <v>-0.547</v>
+        <v>-0.546</v>
       </c>
       <c r="O25" s="1">
-        <v>-0.546</v>
+        <v>-0.545</v>
       </c>
       <c r="P25" s="1">
-        <v>-0.512</v>
+        <v>-0.51</v>
       </c>
       <c r="Q25" s="1">
-        <v>-0.447</v>
+        <v>-0.446</v>
       </c>
       <c r="R25" s="1">
-        <v>-0.351</v>
+        <v>-0.35</v>
       </c>
       <c r="S25" s="1">
-        <v>-0.221</v>
+        <v>-0.22</v>
       </c>
       <c r="T25" s="1">
-        <v>-0.081</v>
+        <v>-0.08</v>
       </c>
       <c r="U25" s="1">
-        <v>0.028</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -2144,46 +2147,46 @@
         <v>-0.458</v>
       </c>
       <c r="H26" s="1">
-        <v>-0.5620000000000001</v>
+        <v>-0.5610000000000001</v>
       </c>
       <c r="I26" s="1">
-        <v>-0.625</v>
+        <v>-0.624</v>
       </c>
       <c r="J26" s="1">
-        <v>-0.643</v>
+        <v>-0.642</v>
       </c>
       <c r="K26" s="1">
-        <v>-0.67</v>
+        <v>-0.669</v>
       </c>
       <c r="L26" s="1">
-        <v>-0.733</v>
+        <v>-0.732</v>
       </c>
       <c r="M26" s="1">
-        <v>-0.795</v>
+        <v>-0.794</v>
       </c>
       <c r="N26" s="1">
-        <v>-0.804</v>
+        <v>-0.803</v>
       </c>
       <c r="O26" s="1">
-        <v>-0.747</v>
+        <v>-0.745</v>
       </c>
       <c r="P26" s="1">
-        <v>-0.647</v>
+        <v>-0.646</v>
       </c>
       <c r="Q26" s="1">
-        <v>-0.521</v>
+        <v>-0.52</v>
       </c>
       <c r="R26" s="1">
-        <v>-0.364</v>
+        <v>-0.363</v>
       </c>
       <c r="S26" s="1">
-        <v>-0.193</v>
+        <v>-0.192</v>
       </c>
       <c r="T26" s="1">
-        <v>-0.053</v>
+        <v>-0.052</v>
       </c>
       <c r="U26" s="1">
-        <v>0.033</v>
+        <v>0.034</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -2206,49 +2209,49 @@
         <v>-0.283</v>
       </c>
       <c r="G27" s="1">
-        <v>-0.409</v>
+        <v>-0.408</v>
       </c>
       <c r="H27" s="1">
-        <v>-0.481</v>
+        <v>-0.48</v>
       </c>
       <c r="I27" s="1">
         <v>-0.504</v>
       </c>
       <c r="J27" s="1">
-        <v>-0.532</v>
+        <v>-0.531</v>
       </c>
       <c r="K27" s="1">
-        <v>-0.585</v>
+        <v>-0.584</v>
       </c>
       <c r="L27" s="1">
-        <v>-0.638</v>
+        <v>-0.637</v>
       </c>
       <c r="M27" s="1">
-        <v>-0.65</v>
+        <v>-0.649</v>
       </c>
       <c r="N27" s="1">
-        <v>-0.603</v>
+        <v>-0.602</v>
       </c>
       <c r="O27" s="1">
-        <v>-0.513</v>
+        <v>-0.512</v>
       </c>
       <c r="P27" s="1">
-        <v>-0.402</v>
+        <v>-0.401</v>
       </c>
       <c r="Q27" s="1">
-        <v>-0.276</v>
+        <v>-0.275</v>
       </c>
       <c r="R27" s="1">
-        <v>-0.152</v>
+        <v>-0.151</v>
       </c>
       <c r="S27" s="1">
-        <v>-0.06</v>
+        <v>-0.059</v>
       </c>
       <c r="T27" s="1">
-        <v>-0.008999999999999999</v>
+        <v>-0.008</v>
       </c>
       <c r="U27" s="1">
-        <v>0.021</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -2268,52 +2271,52 @@
         <v>-0.029</v>
       </c>
       <c r="F28" s="1">
-        <v>-0.147</v>
+        <v>-0.146</v>
       </c>
       <c r="G28" s="1">
-        <v>-0.226</v>
+        <v>-0.225</v>
       </c>
       <c r="H28" s="1">
-        <v>-0.267</v>
+        <v>-0.266</v>
       </c>
       <c r="I28" s="1">
-        <v>-0.301</v>
+        <v>-0.3</v>
       </c>
       <c r="J28" s="1">
-        <v>-0.343</v>
+        <v>-0.342</v>
       </c>
       <c r="K28" s="1">
-        <v>-0.383</v>
+        <v>-0.382</v>
       </c>
       <c r="L28" s="1">
-        <v>-0.399</v>
+        <v>-0.397</v>
       </c>
       <c r="M28" s="1">
-        <v>-0.374</v>
+        <v>-0.372</v>
       </c>
       <c r="N28" s="1">
-        <v>-0.316</v>
+        <v>-0.315</v>
       </c>
       <c r="O28" s="1">
-        <v>-0.245</v>
+        <v>-0.244</v>
       </c>
       <c r="P28" s="1">
-        <v>-0.176</v>
+        <v>-0.175</v>
       </c>
       <c r="Q28" s="1">
-        <v>-0.118</v>
+        <v>-0.117</v>
       </c>
       <c r="R28" s="1">
-        <v>-0.082</v>
+        <v>-0.081</v>
       </c>
       <c r="S28" s="1">
-        <v>-0.066</v>
+        <v>-0.065</v>
       </c>
       <c r="T28" s="1">
         <v>-0.058</v>
       </c>
       <c r="U28" s="1">
-        <v>-0.048</v>
+        <v>-0.047</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -2330,49 +2333,49 @@
         <v>-0.115</v>
       </c>
       <c r="E29" s="1">
-        <v>-0.144</v>
+        <v>-0.143</v>
       </c>
       <c r="F29" s="1">
+        <v>-0.156</v>
+      </c>
+      <c r="G29" s="1">
         <v>-0.157</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <v>-0.158</v>
       </c>
-      <c r="H29" s="1">
-        <v>-0.159</v>
-      </c>
       <c r="I29" s="1">
-        <v>-0.156</v>
+        <v>-0.154</v>
       </c>
       <c r="J29" s="1">
-        <v>-0.148</v>
+        <v>-0.146</v>
       </c>
       <c r="K29" s="1">
-        <v>-0.141</v>
+        <v>-0.139</v>
       </c>
       <c r="L29" s="1">
-        <v>-0.131</v>
+        <v>-0.13</v>
       </c>
       <c r="M29" s="1">
-        <v>-0.108</v>
+        <v>-0.107</v>
       </c>
       <c r="N29" s="1">
-        <v>-0.068</v>
+        <v>-0.067</v>
       </c>
       <c r="O29" s="1">
-        <v>-0.018</v>
+        <v>-0.017</v>
       </c>
       <c r="P29" s="1">
         <v>0.026</v>
       </c>
       <c r="Q29" s="1">
+        <v>0.049</v>
+      </c>
+      <c r="R29" s="1">
+        <v>0.051</v>
+      </c>
+      <c r="S29" s="1">
         <v>0.048</v>
-      </c>
-      <c r="R29" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="S29" s="1">
-        <v>0.047</v>
       </c>
       <c r="T29" s="1">
         <v>0.056</v>
@@ -2395,43 +2398,43 @@
         <v>-0.081</v>
       </c>
       <c r="E30" s="1">
-        <v>-0.103</v>
+        <v>-0.102</v>
       </c>
       <c r="F30" s="1">
-        <v>-0.119</v>
+        <v>-0.118</v>
       </c>
       <c r="G30" s="1">
-        <v>-0.145</v>
+        <v>-0.144</v>
       </c>
       <c r="H30" s="1">
-        <v>-0.182</v>
+        <v>-0.18</v>
       </c>
       <c r="I30" s="1">
-        <v>-0.216</v>
+        <v>-0.214</v>
       </c>
       <c r="J30" s="1">
-        <v>-0.233</v>
+        <v>-0.231</v>
       </c>
       <c r="K30" s="1">
-        <v>-0.221</v>
+        <v>-0.22</v>
       </c>
       <c r="L30" s="1">
-        <v>-0.184</v>
+        <v>-0.183</v>
       </c>
       <c r="M30" s="1">
-        <v>-0.143</v>
+        <v>-0.142</v>
       </c>
       <c r="N30" s="1">
+        <v>-0.115</v>
+      </c>
+      <c r="O30" s="1">
+        <v>-0.105</v>
+      </c>
+      <c r="P30" s="1">
+        <v>-0.108</v>
+      </c>
+      <c r="Q30" s="1">
         <v>-0.116</v>
-      </c>
-      <c r="O30" s="1">
-        <v>-0.106</v>
-      </c>
-      <c r="P30" s="1">
-        <v>-0.109</v>
-      </c>
-      <c r="Q30" s="1">
-        <v>-0.117</v>
       </c>
       <c r="R30" s="1">
         <v>-0.123</v>
@@ -2440,10 +2443,10 @@
         <v>-0.131</v>
       </c>
       <c r="T30" s="1">
-        <v>-0.143</v>
+        <v>-0.142</v>
       </c>
       <c r="U30" s="1">
-        <v>-0.152</v>
+        <v>-0.151</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -2454,58 +2457,58 @@
         <v>0.024</v>
       </c>
       <c r="C31" s="1">
-        <v>-0.002</v>
+        <v>-0.001</v>
       </c>
       <c r="D31" s="1">
-        <v>-0.038</v>
+        <v>-0.037</v>
       </c>
       <c r="E31" s="1">
-        <v>-0.062</v>
+        <v>-0.061</v>
       </c>
       <c r="F31" s="1">
-        <v>-0.107</v>
+        <v>-0.106</v>
       </c>
       <c r="G31" s="1">
-        <v>-0.187</v>
+        <v>-0.185</v>
       </c>
       <c r="H31" s="1">
-        <v>-0.267</v>
+        <v>-0.266</v>
       </c>
       <c r="I31" s="1">
+        <v>-0.301</v>
+      </c>
+      <c r="J31" s="1">
+        <v>-0.277</v>
+      </c>
+      <c r="K31" s="1">
+        <v>-0.227</v>
+      </c>
+      <c r="L31" s="1">
+        <v>-0.199</v>
+      </c>
+      <c r="M31" s="1">
+        <v>-0.218</v>
+      </c>
+      <c r="N31" s="1">
+        <v>-0.264</v>
+      </c>
+      <c r="O31" s="1">
         <v>-0.303</v>
       </c>
-      <c r="J31" s="1">
-        <v>-0.279</v>
-      </c>
-      <c r="K31" s="1">
-        <v>-0.228</v>
-      </c>
-      <c r="L31" s="1">
-        <v>-0.201</v>
-      </c>
-      <c r="M31" s="1">
-        <v>-0.219</v>
-      </c>
-      <c r="N31" s="1">
-        <v>-0.265</v>
-      </c>
-      <c r="O31" s="1">
-        <v>-0.304</v>
-      </c>
       <c r="P31" s="1">
-        <v>-0.319</v>
+        <v>-0.318</v>
       </c>
       <c r="Q31" s="1">
         <v>-0.319</v>
       </c>
       <c r="R31" s="1">
-        <v>-0.34</v>
+        <v>-0.339</v>
       </c>
       <c r="S31" s="1">
-        <v>-0.393</v>
+        <v>-0.392</v>
       </c>
       <c r="T31" s="1">
-        <v>-0.449</v>
+        <v>-0.448</v>
       </c>
       <c r="U31" s="1">
         <v>-0.463</v>
@@ -2516,64 +2519,129 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>-0.046</v>
+        <v>-0.062</v>
       </c>
       <c r="C32" s="1">
-        <v>-0.08</v>
+        <v>-0.096</v>
       </c>
       <c r="D32" s="1">
-        <v>-0.143</v>
+        <v>-0.16</v>
       </c>
       <c r="E32" s="1">
-        <v>-0.229</v>
+        <v>-0.247</v>
       </c>
       <c r="F32" s="1">
-        <v>-0.345</v>
+        <v>-0.365</v>
       </c>
       <c r="G32" s="1">
-        <v>-0.449</v>
+        <v>-0.469</v>
       </c>
       <c r="H32" s="1">
-        <v>-0.49</v>
+        <v>-0.509</v>
       </c>
       <c r="I32" s="1">
-        <v>-0.457</v>
+        <v>-0.474</v>
       </c>
       <c r="J32" s="1">
-        <v>-0.381</v>
+        <v>-0.396</v>
       </c>
       <c r="K32" s="1">
-        <v>-0.32</v>
+        <v>-0.332</v>
       </c>
       <c r="L32" s="1">
-        <v>-0.306</v>
+        <v>-0.312</v>
       </c>
       <c r="M32" s="1">
         <v>-0.326</v>
       </c>
       <c r="N32" s="1">
-        <v>-0.353</v>
+        <v>-0.347</v>
       </c>
       <c r="O32" s="1">
-        <v>-0.364</v>
+        <v>-0.355</v>
       </c>
       <c r="P32" s="1">
-        <v>-0.364</v>
+        <v>-0.354</v>
       </c>
       <c r="Q32" s="1">
-        <v>-0.384</v>
+        <v>-0.373</v>
       </c>
       <c r="R32" s="1">
-        <v>-0.436</v>
+        <v>-0.422</v>
       </c>
       <c r="S32" s="1">
-        <v>-0.489</v>
+        <v>-0.472</v>
       </c>
       <c r="T32" s="1">
-        <v>-0.504</v>
+        <v>-0.486</v>
       </c>
       <c r="U32" s="1">
-        <v>-0.471</v>
+        <v>-0.455</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>-0.332</v>
+      </c>
+      <c r="C33" s="1">
+        <v>-0.352</v>
+      </c>
+      <c r="D33" s="1">
+        <v>-0.432</v>
+      </c>
+      <c r="E33" s="1">
+        <v>-0.5610000000000001</v>
+      </c>
+      <c r="F33" s="1">
+        <v>-0.663</v>
+      </c>
+      <c r="G33" s="1">
+        <v>-0.678</v>
+      </c>
+      <c r="H33" s="1">
+        <v>-0.612</v>
+      </c>
+      <c r="I33" s="1">
+        <v>-0.511</v>
+      </c>
+      <c r="J33" s="1">
+        <v>-0.417</v>
+      </c>
+      <c r="K33" s="1">
+        <v>-0.348</v>
+      </c>
+      <c r="L33" s="1">
+        <v>-0.302</v>
+      </c>
+      <c r="M33" s="1">
+        <v>-0.272</v>
+      </c>
+      <c r="N33" s="1">
+        <v>-0.255</v>
+      </c>
+      <c r="O33" s="1">
+        <v>-0.242</v>
+      </c>
+      <c r="P33" s="1">
+        <v>-0.243</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>-0.261</v>
+      </c>
+      <c r="R33" s="1">
+        <v>-0.279</v>
+      </c>
+      <c r="S33" s="1">
+        <v>-0.282</v>
+      </c>
+      <c r="T33" s="1">
+        <v>-0.273</v>
+      </c>
+      <c r="U33" s="1">
+        <v>-0.247</v>
       </c>
     </row>
   </sheetData>
@@ -2591,22 +2659,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
XRO forecast & update cv
</commit_message>
<xml_diff>
--- a/content/climate/XRO/XRO_ENSO_fcst.xlsx
+++ b/content/climate/XRO/XRO_ENSO_fcst.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>init</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>2025-08</t>
+  </si>
+  <si>
+    <t>2025-09</t>
   </si>
   <si>
     <t>Readme</t>
@@ -490,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -501,7 +504,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2">
         <v>0</v>
@@ -2525,58 +2528,58 @@
         <v>-0.096</v>
       </c>
       <c r="D32" s="1">
-        <v>-0.16</v>
+        <v>-0.159</v>
       </c>
       <c r="E32" s="1">
-        <v>-0.247</v>
+        <v>-0.246</v>
       </c>
       <c r="F32" s="1">
-        <v>-0.365</v>
+        <v>-0.364</v>
       </c>
       <c r="G32" s="1">
-        <v>-0.469</v>
+        <v>-0.467</v>
       </c>
       <c r="H32" s="1">
-        <v>-0.509</v>
+        <v>-0.507</v>
       </c>
       <c r="I32" s="1">
-        <v>-0.474</v>
+        <v>-0.472</v>
       </c>
       <c r="J32" s="1">
-        <v>-0.396</v>
+        <v>-0.395</v>
       </c>
       <c r="K32" s="1">
-        <v>-0.332</v>
+        <v>-0.331</v>
       </c>
       <c r="L32" s="1">
-        <v>-0.312</v>
+        <v>-0.311</v>
       </c>
       <c r="M32" s="1">
-        <v>-0.326</v>
+        <v>-0.325</v>
       </c>
       <c r="N32" s="1">
-        <v>-0.347</v>
+        <v>-0.346</v>
       </c>
       <c r="O32" s="1">
-        <v>-0.355</v>
+        <v>-0.354</v>
       </c>
       <c r="P32" s="1">
-        <v>-0.354</v>
+        <v>-0.353</v>
       </c>
       <c r="Q32" s="1">
-        <v>-0.373</v>
+        <v>-0.372</v>
       </c>
       <c r="R32" s="1">
-        <v>-0.422</v>
+        <v>-0.421</v>
       </c>
       <c r="S32" s="1">
-        <v>-0.472</v>
+        <v>-0.471</v>
       </c>
       <c r="T32" s="1">
-        <v>-0.486</v>
+        <v>-0.484</v>
       </c>
       <c r="U32" s="1">
-        <v>-0.455</v>
+        <v>-0.454</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -2584,64 +2587,129 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <v>-0.332</v>
+        <v>-0.306</v>
       </c>
       <c r="C33" s="1">
-        <v>-0.352</v>
+        <v>-0.33</v>
       </c>
       <c r="D33" s="1">
-        <v>-0.432</v>
+        <v>-0.417</v>
       </c>
       <c r="E33" s="1">
-        <v>-0.5610000000000001</v>
+        <v>-0.548</v>
       </c>
       <c r="F33" s="1">
-        <v>-0.663</v>
+        <v>-0.652</v>
       </c>
       <c r="G33" s="1">
-        <v>-0.678</v>
+        <v>-0.669</v>
       </c>
       <c r="H33" s="1">
-        <v>-0.612</v>
+        <v>-0.605</v>
       </c>
       <c r="I33" s="1">
-        <v>-0.511</v>
+        <v>-0.505</v>
       </c>
       <c r="J33" s="1">
-        <v>-0.417</v>
+        <v>-0.412</v>
       </c>
       <c r="K33" s="1">
-        <v>-0.348</v>
+        <v>-0.346</v>
       </c>
       <c r="L33" s="1">
-        <v>-0.302</v>
+        <v>-0.301</v>
       </c>
       <c r="M33" s="1">
-        <v>-0.272</v>
+        <v>-0.275</v>
       </c>
       <c r="N33" s="1">
-        <v>-0.255</v>
+        <v>-0.258</v>
       </c>
       <c r="O33" s="1">
-        <v>-0.242</v>
+        <v>-0.247</v>
       </c>
       <c r="P33" s="1">
-        <v>-0.243</v>
+        <v>-0.249</v>
       </c>
       <c r="Q33" s="1">
-        <v>-0.261</v>
+        <v>-0.269</v>
       </c>
       <c r="R33" s="1">
-        <v>-0.279</v>
+        <v>-0.288</v>
       </c>
       <c r="S33" s="1">
-        <v>-0.282</v>
+        <v>-0.291</v>
       </c>
       <c r="T33" s="1">
-        <v>-0.273</v>
+        <v>-0.281</v>
       </c>
       <c r="U33" s="1">
-        <v>-0.247</v>
+        <v>-0.254</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
+        <v>-0.42</v>
+      </c>
+      <c r="C34" s="1">
+        <v>-0.478</v>
+      </c>
+      <c r="D34" s="1">
+        <v>-0.599</v>
+      </c>
+      <c r="E34" s="1">
+        <v>-0.7</v>
+      </c>
+      <c r="F34" s="1">
+        <v>-0.725</v>
+      </c>
+      <c r="G34" s="1">
+        <v>-0.666</v>
+      </c>
+      <c r="H34" s="1">
+        <v>-0.5600000000000001</v>
+      </c>
+      <c r="I34" s="1">
+        <v>-0.451</v>
+      </c>
+      <c r="J34" s="1">
+        <v>-0.366</v>
+      </c>
+      <c r="K34" s="1">
+        <v>-0.305</v>
+      </c>
+      <c r="L34" s="1">
+        <v>-0.269</v>
+      </c>
+      <c r="M34" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="N34" s="1">
+        <v>-0.238</v>
+      </c>
+      <c r="O34" s="1">
+        <v>-0.237</v>
+      </c>
+      <c r="P34" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>-0.262</v>
+      </c>
+      <c r="R34" s="1">
+        <v>-0.264</v>
+      </c>
+      <c r="S34" s="1">
+        <v>-0.258</v>
+      </c>
+      <c r="T34" s="1">
+        <v>-0.236</v>
+      </c>
+      <c r="U34" s="1">
+        <v>-0.186</v>
       </c>
     </row>
   </sheetData>
@@ -2659,22 +2727,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>